<commit_message>
No video links in activity description in chat (only in reminder message)
</commit_message>
<xml_diff>
--- a/Activities.xlsx
+++ b/Activities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\Documents\PerfectFitt\First Experiment\Activities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9522FDF-FF08-40A6-B9F1-3BE2CDDD8C56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF66B150-675E-463B-96F8-BFAF49319E24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activities" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="212">
   <si>
     <t>Number</t>
   </si>
@@ -67,9 +67,6 @@
     <t>Exclusion</t>
   </si>
   <si>
-    <t>Formulation</t>
-  </si>
-  <si>
     <t>Behavior Goal</t>
   </si>
   <si>
@@ -641,6 +638,24 @@
   </si>
   <si>
     <t>record my current physical activity routines</t>
+  </si>
+  <si>
+    <t>Formulation Email</t>
+  </si>
+  <si>
+    <t>Formulation Chat</t>
+  </si>
+  <si>
+    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, between this and the next session, please watch the 15-minute video that I will send you as a message in Prolific. The video will help you to learn progressive muscle relaxation (which is a way of relaxing your body). Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
+  </si>
+  <si>
+    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, between this and the next session, please watch the 12-minute video that I will send you as a message in Prolific. The video explains how the body starts repairing itself immediately, as soon as a person stops smoking. What information from the video is most relevant to you? Take a few notes.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, between this and the next session, please watch the 2-minute video that I will send you as a message in Prolific. The video explains how much and which type of physical activity is recommended. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, between this and the next session, please watch the 5-minute video that I will send you as a message in Prolific. The video explains the possible positive impact of physical activity on dealing with cravings to smoke. What do you think about the information in the video? Write down your thoughts in a few words.</t>
   </si>
 </sst>
 </file>
@@ -1484,20 +1499,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="I24" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="16" width="10.77734375" customWidth="1"/>
-    <col min="17" max="17" width="33.77734375" customWidth="1"/>
-    <col min="18" max="18" width="10.77734375" customWidth="1"/>
+    <col min="17" max="18" width="33.77734375" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1505,7 +1520,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1547,1268 +1562,1343 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:18" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>29</v>
-      </c>
     </row>
-    <row r="3" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>29</v>
+        <v>165</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>29</v>
+        <v>164</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="216" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="216" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>29</v>
+        <v>163</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="M6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>29</v>
+        <v>166</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="L7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>29</v>
+        <v>167</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="L8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="L8" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="O8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>29</v>
+        <v>169</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="216" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="216" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="L9" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>29</v>
+        <v>173</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G10" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="L10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>180</v>
+        <v>208</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>29</v>
+        <v>179</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="K11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="L11" s="1" t="s">
+      <c r="M11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>29</v>
+        <v>172</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>172</v>
+        <v>209</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>29</v>
+        <v>171</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="L13" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="L13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>29</v>
+        <v>197</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="J14" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>206</v>
-      </c>
       <c r="L14" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>95</v>
+        <v>190</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>95</v>
+        <v>191</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="G16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="L16" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="L16" s="1" t="s">
+      <c r="M16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>95</v>
+        <v>180</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="288" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="288" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="L17" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="P17" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="Q17" s="1" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>95</v>
+        <v>181</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>95</v>
+        <v>182</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>95</v>
+        <v>192</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="288" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="288" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>95</v>
+        <v>193</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="G21" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H21" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>138</v>
-      </c>
       <c r="L21" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>95</v>
+        <v>194</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="259.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="L22" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>95</v>
+        <v>185</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="G23" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="L23" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>95</v>
+        <v>195</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="G24" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="L24" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>95</v>
+        <v>196</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="G25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="L25" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>95</v>
+        <v>186</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed activity formulation for reminder email to say before the next session only
</commit_message>
<xml_diff>
--- a/Activities.xlsx
+++ b/Activities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\Documents\PerfectFitt\First Experiment\Activities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0311D80F-63BE-49B6-BE74-297390E6A17E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA51C8C-579D-4DC1-9E60-33CBF720E8B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="232">
   <si>
     <t>Number</t>
   </si>
@@ -535,9 +535,6 @@
     <t>may make it HARDER to refrain from smoking</t>
   </si>
   <si>
-    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, between this and the next session, please watch the following 12-minute video on how the body starts repairing itself immediately, as soon as a person stops smoking: https://www.youtube.com/watch?v=ZhTOC0T3P3c&amp;ab_channel=RespiratoryTherapyZone. What information from the video is most relevant to you? Take a few notes.</t>
-  </si>
-  <si>
     <t>Having strong determination to refrain from smoking may help to quit successfully. So, between this and the next session, please take some time to think of a personal rule that helps you to refrain from smoking. Possible examples include "Not a puff - no matter what,” "Say no to smoking, yes to life" or "Smoking is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
   </si>
   <si>
@@ -559,15 +556,9 @@
     <t>may make it HARD to prepare for and thus resist cravings to smoke</t>
   </si>
   <si>
-    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, between this and the next session, please watch the following 15-minute video to learn progressive muscle relaxation (which is a way of relaxing your body): https://www.youtube.com/watch?v=ihO02wUzgkc&amp;ab_channel=MarkConnelly. Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
-  </si>
-  <si>
     <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have a strong desire to become more physically active. Therefore, between this and the next session, please identify and write down reasons why you want to become more physically active. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
   </si>
   <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, between this and the next session, please watch the following 2-minute video on how much and which type of physical activity is recommended: https://www.youtube.com/watch?v=AAPhWbG_zLs&amp;ab_channel=TREKGroup. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
-  </si>
-  <si>
     <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for this is to have high ambition to become more physically active. Thus, between this and the next session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
   </si>
   <si>
@@ -604,9 +595,6 @@
     <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, between this and the next session, please think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
   </si>
   <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, between this and the next session, please watch the following 5-minute video about the possible positive impact of physical activity on dealing with cravings to smoke: https://www.youtube.com/watch?v=StM10jzbt1k&amp;ab_channel=TreeHouseRecovery. What do you think about the information in the video? Write down your thoughts in a few words.</t>
-  </si>
-  <si>
     <t>Preparing for situations in which you commonly smoke may make it easier to successfully quit smoking. Therefore, please record the situations in which you smoke between this and the next session. Take note of one or two keywords to describe the situation and the number of cigarettes that you smoked. For example, you might note "Lunch break, 2 cigarettes" or "TV, 5 cigarettes." It might be helpful to take these notes on your phone, or you could carry a small piece of paper and pen in your pocket.</t>
   </si>
   <si>
@@ -656,6 +644,78 @@
   </si>
   <si>
     <t>Becoming more physically active (e.g. exercise, take walks, sit less) may make it easier to successfully quit smoking. One important step for becoming more physically active is to know one's current level. This allows to later set a precise goal and hence to feel more motivated. So, please record your current behavior with regards to physical activity between this and the next session. Try to keep track of how much time you spend 1) sitting, 2) working out and 3) being moderately active (e.g. taking a walk, biking to the grocery store). For this, it might be helpful to keep a piece of paper and pen on your kitchen table, or maybe you have a smart watch that can record these types of behavior for you.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, before the next session, please watch the following 2-minute video on how much and which type of physical activity is recommended: https://www.youtube.com/watch?v=AAPhWbG_zLs&amp;ab_channel=TREKGroup. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for this is to have high ambition to become more physically active. Thus, before the next session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, before the next session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Write down everything that comes to your mind. </t>
+  </si>
+  <si>
+    <t>It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, before the next session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Then, look for a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for this is to focus on the goal of becoming more physically active. Thus, before the next session, please take some time to visualize becoming more physically active as a battle. For example, you might see yourself and non-active version of yourself as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high motivation to become more physically active. Thus, before the next session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Then look for a picture that best captures your desired future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, before the next session, please think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, before the next session, please watch the following 5-minute video about the possible positive impact of physical activity on dealing with cravings to smoke: https://www.youtube.com/watch?v=StM10jzbt1k&amp;ab_channel=TreeHouseRecovery. What do you think about the information in the video? Write down your thoughts in a few words.</t>
+  </si>
+  <si>
+    <t>Being more physically active (e.g. exercise, take walks, spend less time sitting) may aid you to stop smoking. One important aspect for this is to have strong resolve to become more physically active. So, before the next session, please take some time to think of a personal rule that helps you to become more physically active. Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have a strong desire to become more physically active. Therefore, before the next session, please identify and write down reasons why you want to become more physically active. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for becoming more physically active is to remove possible obstacles. Thus, before the next session, please think about things that make it difficult for you to be physically active. For example, this could be that you do NOT have a raincoat to bike to the grocery store when it is raining, that you do NOT want to work out alone, or that you are at work all day and too exhausted by the time that you come home. What are possible solutions to your barriers? For instance, you could buy a raincoat, join a running group, or take a walk during your lunch break at work. Please write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may make it easier to successfully quit smoking. One important step for becoming more physically active is to know one's current level. This allows to later set a precise goal and hence to feel more motivated. So, please record your current behavior with regards to physical activity before the next session. Try to keep track of how much time you spend 1) sitting, 2) working out and 3) being moderately active (e.g. taking a walk, biking to the grocery store). For this, it might be helpful to keep a piece of paper and pen on your kitchen table, or maybe you have a smart watch that can record these types of behavior for you.</t>
+  </si>
+  <si>
+    <t>Preparing for situations in which you commonly smoke may make it easier to successfully quit smoking. Therefore, please record the situations in which you smoke before the next session. Take note of one or two keywords to describe the situation and the number of cigarettes that you smoked. For example, you might note "Lunch break, 2 cigarettes" or "TV, 5 cigarettes." It might be helpful to take these notes on your phone, or you could carry a small piece of paper and pen in your pocket.</t>
+  </si>
+  <si>
+    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, before the next session, please watch the following 12-minute video on how the body starts repairing itself immediately, as soon as a person stops smoking: https://www.youtube.com/watch?v=ZhTOC0T3P3c&amp;ab_channel=RespiratoryTherapyZone. What information from the video is most relevant to you? Take a few notes.</t>
+  </si>
+  <si>
+    <t>Having strong determination to refrain from smoking may help to quit successfully. So, before the next session, please take some time to think of a personal rule that helps you to refrain from smoking. Possible examples include "Not a puff - no matter what,” "Say no to smoking, yes to life" or "Smoking is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
+  </si>
+  <si>
+    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, before the next session, please watch the following 15-minute video to learn progressive muscle relaxation (which is a way of relaxing your body): https://www.youtube.com/watch?v=ihO02wUzgkc&amp;ab_channel=MarkConnelly. Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
+  </si>
+  <si>
+    <t>Planning how to resist urges to smoke may make it easier to successfully quit smoking. Therefore, before the next session, please think of activities that you could do to keep yourself busy when you feel the urge to smoke so that you do NOT smoke. These urges typically last a few minutes; think of something that you could do in the meantime until the urge has passed. For example, you could water your plants, eat a carrot, do 10 push-ups, or do something for another person in need. Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Preparing for situations in which avoiding to smoke is difficult may make it easier to successfully quit smoking. Thus, before the next session, please think about situations in which you might find it difficult to refrain from smoking. For example, this could be during your lunch break at work, when you meet your best friend, or when you watch TV. How could you deal with these situations so that you do NOT smoke? Write down your plans in a few words.</t>
+  </si>
+  <si>
+    <t>Getting fewer cravings to smoke may make it easier to successfully quit smoking. Therefore, before the next session, please think about routines in your daily life that often cause you to get cravings to smoke. For example, you might have experienced that if you go to bed very late and thus sleep less, you smoke more the next day. Or maybe you have noticed that if you skip your breakfast, you always smoke on your way to work but NOT otherwise. How could you change these routines to reduce or even avoid those cravings? Please write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Focusing on your goal of successfully quitting smoking may help to quit. Thus, before the next session, please take some time to visualize smoking as a battle. For example, you might see yourself and a cigarette as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
+  </si>
+  <si>
+    <t>Having high motivation to quit smoking may help to quit successfully. So, before the next session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Then, look for or take a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having high motivation to quit smoking may aid quitting successfully. Thus, before the next session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Write down everything that comes to your mind. </t>
+  </si>
+  <si>
+    <t>Having high aspiration to quit smoking may aid quitting successfully. So, before the next session, please identify and write down reasons why you want to stop smoking. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
+  </si>
+  <si>
+    <t>Having high aspiration to quit smoking may aid quitting successfully. Thus, before the next session, please think about the person that you would like to be once you have successfully quit smoking. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
   </si>
 </sst>
 </file>
@@ -1501,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I14" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1562,10 +1622,10 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>15</v>
@@ -1582,7 +1642,7 @@
         <v>158</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
@@ -1619,10 +1679,10 @@
         <v>27</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>198</v>
+        <v>231</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>28</v>
@@ -1677,7 +1737,7 @@
         <v>165</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>165</v>
+        <v>230</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>28</v>
@@ -1718,13 +1778,13 @@
         <v>43</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
@@ -1734,7 +1794,7 @@
         <v>164</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>164</v>
+        <v>229</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>28</v>
@@ -1775,13 +1835,13 @@
         <v>43</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
@@ -1791,7 +1851,7 @@
         <v>163</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>163</v>
+        <v>228</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>28</v>
@@ -1846,7 +1906,7 @@
         <v>166</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>28</v>
@@ -1887,7 +1947,7 @@
         <v>162</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>34</v>
@@ -1903,7 +1963,7 @@
         <v>167</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>167</v>
+        <v>226</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>28</v>
@@ -1960,7 +2020,7 @@
         <v>169</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>169</v>
+        <v>225</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>28</v>
@@ -2001,7 +2061,7 @@
         <v>64</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>34</v>
@@ -2012,16 +2072,16 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>173</v>
+        <v>224</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -2056,23 +2116,23 @@
         <v>69</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
         <v>70</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>179</v>
+        <v>223</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>28</v>
@@ -2126,10 +2186,10 @@
         <v>76</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>28</v>
@@ -2183,10 +2243,10 @@
         <v>87</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>28</v>
@@ -2227,21 +2287,21 @@
         <v>91</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>92</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>28</v>
@@ -2258,28 +2318,28 @@
         <v>159</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>154</v>
@@ -2291,10 +2351,10 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>94</v>
@@ -2344,10 +2404,10 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>189</v>
+        <v>218</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>94</v>
@@ -2399,16 +2459,16 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="288" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2456,10 +2516,10 @@
         <v>118</v>
       </c>
       <c r="Q17" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="R17" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="R17" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>94</v>
@@ -2511,10 +2571,10 @@
         <v>125</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>182</v>
+        <v>209</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>94</v>
@@ -2566,10 +2626,10 @@
         <v>132</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>94</v>
@@ -2621,10 +2681,10 @@
         <v>133</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>94</v>
@@ -2665,19 +2725,19 @@
         <v>137</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>94</v>
@@ -2729,10 +2789,10 @@
         <v>140</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>185</v>
+        <v>213</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>94</v>
@@ -2782,10 +2842,10 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>94</v>
@@ -2802,28 +2862,28 @@
         <v>159</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>147</v>
@@ -2837,10 +2897,10 @@
         <v>149</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>194</v>
+        <v>215</v>
       </c>
       <c r="S24" s="1" t="s">
         <v>94</v>
@@ -2892,10 +2952,10 @@
         <v>152</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="S25" s="1" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
make prerequisite and exclusion indices in activities.csv start from 0 rather than 1
</commit_message>
<xml_diff>
--- a/Activities.xlsx
+++ b/Activities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\Documents\PerfectFitt\First Experiment\Activities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\CAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58159750-08E5-43DA-8AAF-F5C0A0BE7857}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A2870F-8481-4A97-B768-0D0C6DFEA2C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,9 +103,6 @@
     <t>may lead to INSUFFICIENT aspiration to move away from smoking</t>
   </si>
   <si>
-    <t>17,21</t>
-  </si>
-  <si>
     <t>quit smoking</t>
   </si>
   <si>
@@ -154,12 +151,6 @@
     <t>think about who I do NOT want to be but might become if I continue to smoke</t>
   </si>
   <si>
-    <t>4,19,18</t>
-  </si>
-  <si>
-    <t>3,19,18</t>
-  </si>
-  <si>
     <t>visualizing smoking as a battle that you win</t>
   </si>
   <si>
@@ -250,9 +241,6 @@
     <t>may lead to INSUFFICIENT determination to refrain from smoking</t>
   </si>
   <si>
-    <t>24,</t>
-  </si>
-  <si>
     <t>learning about how your body starts repairing itself as soon as you stop smoking</t>
   </si>
   <si>
@@ -283,439 +271,451 @@
     <t>may lead to a LACK of desire to refrain from smoking</t>
   </si>
   <si>
+    <t>recording your current smoking behavior</t>
+  </si>
+  <si>
+    <t>Recording your current smoking behavior</t>
+  </si>
+  <si>
+    <t>record your current smoking behavior</t>
+  </si>
+  <si>
+    <t>record my current smoking behavior</t>
+  </si>
+  <si>
+    <t>None, but helps for the activities that ask to come up with routines etc.</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>become more physically active</t>
+  </si>
+  <si>
+    <t>thinking about solutions to possible barriers</t>
+  </si>
+  <si>
+    <t>thinking about solutions to barriers</t>
+  </si>
+  <si>
+    <t>Thinking about solutions to barriers</t>
+  </si>
+  <si>
+    <t>think about solutions to barriers</t>
+  </si>
+  <si>
+    <t>Thinking about solutions to possible barriers</t>
+  </si>
+  <si>
+    <t>think about solutions to possible barriers</t>
+  </si>
+  <si>
+    <t>REMOVE obstacles to becoming more physically active</t>
+  </si>
+  <si>
+    <t>may cause those barriers to PREVENT you from becoming more physically active</t>
+  </si>
+  <si>
+    <t>identifying reasons why you want to become more physically active</t>
+  </si>
+  <si>
+    <t>Identifying reasons why you want to become more physically active</t>
+  </si>
+  <si>
+    <t>identify reasons why you want to become more physically active</t>
+  </si>
+  <si>
+    <t>identify reasons why I want to become more physically active</t>
+  </si>
+  <si>
+    <t>increase your DESIRE to become more physically active</t>
+  </si>
+  <si>
+    <t>may lead to a LACK of desire to become more physically active</t>
+  </si>
+  <si>
+    <t>comparing your current physical activity behavior to what is recommended</t>
+  </si>
+  <si>
+    <t>comparing your physical activity behavior to what is recommended</t>
+  </si>
+  <si>
+    <t>Comparing your physical activity behavior to what is recommended</t>
+  </si>
+  <si>
+    <t>compare your physical activity behavior to what is recommended</t>
+  </si>
+  <si>
+    <t>compare my physical activity behavior to what is recommended</t>
+  </si>
+  <si>
+    <t>Comparing your current physical activity behavior to what is recommended</t>
+  </si>
+  <si>
+    <t>compare your current physical activity behavior to what is recommended</t>
+  </si>
+  <si>
+    <t>compare my current physical activity behavior to what is recommended</t>
+  </si>
+  <si>
+    <t>23,</t>
+  </si>
+  <si>
+    <t>thinking about the person you would like to be once you have become more physically active</t>
+  </si>
+  <si>
+    <t>Thinking about the person you would like to be once you have become more physically active</t>
+  </si>
+  <si>
+    <t>think about the person you would like to be once you have become more physically active</t>
+  </si>
+  <si>
+    <t>think about the person I would like to be once I have become more physically active</t>
+  </si>
+  <si>
+    <t>increase your AMBITION to become a more physically active person</t>
+  </si>
+  <si>
+    <t>may lead to a LACK of ambition to become a more physically active person</t>
+  </si>
+  <si>
+    <t>thinking about who you do NOT want to be but might become if you fail to become more physically active</t>
+  </si>
+  <si>
+    <t>Thinking about who you do NOT want to be but might become if you fail to become more physically active</t>
+  </si>
+  <si>
+    <t>think about who you do NOT want to be but might become if you fail to become more physically active</t>
+  </si>
+  <si>
+    <t>think about who I do NOT want to be but might become if I fail to become more physically active</t>
+  </si>
+  <si>
+    <t>heighten your DETERMINATION to become a more physically active person</t>
+  </si>
+  <si>
+    <t>may lead to INSUFFICIENT determination to become a more physically active person</t>
+  </si>
+  <si>
+    <t>visualizing becoming more physically active as a battle that you win</t>
+  </si>
+  <si>
+    <t>Visualizing becoming more physically active as a battle that you win</t>
+  </si>
+  <si>
+    <t>visualize becoming more physically active as a battle that you win</t>
+  </si>
+  <si>
+    <t>visualize becoming more physically active as a battle that I win</t>
+  </si>
+  <si>
+    <t>feel more MOTIVATED to become a more physically active person</t>
+  </si>
+  <si>
+    <t>may lead to INSUFFICIENT motivation to become a more physically active person</t>
+  </si>
+  <si>
+    <t>thinking about what you could do to become more physically active</t>
+  </si>
+  <si>
+    <t>Thinking about what you could do to become more physically active</t>
+  </si>
+  <si>
+    <t>think about what you could do to become more physically active</t>
+  </si>
+  <si>
+    <t>think about what I could do to become more physically active</t>
+  </si>
+  <si>
+    <t>SUCCEED at becoming more physically active</t>
+  </si>
+  <si>
+    <t>may make it DIFFICULT to become more physically active</t>
+  </si>
+  <si>
+    <t>heighten your ASPIRATION to become more physically active</t>
+  </si>
+  <si>
+    <t>may lead to a LACK of aspiration to become more physically active</t>
+  </si>
+  <si>
+    <t>generate strong RESOLVE to become more physically active</t>
+  </si>
+  <si>
+    <t>may lead to INSUFFICIENT resolve to become more physically active</t>
+  </si>
+  <si>
+    <t>10,</t>
+  </si>
+  <si>
+    <t>set a SPECIFIC GOAL and thus to feel more ASPIRATION to become more physically active</t>
+  </si>
+  <si>
+    <t>set a PRECISE GOAL and thus to feel more MOTIVATED to become more physically active</t>
+  </si>
+  <si>
+    <t>may make it DIFFICULT to set a precise goal and thus lead to INSUFFICIENT motivation to become more physically active</t>
+  </si>
+  <si>
+    <t>may make it HARD to set a specific goal and thus lead to INSUFFICIENT aspiration to become more physically active</t>
+  </si>
+  <si>
+    <t>Experts</t>
+  </si>
+  <si>
+    <t>Smoking cessation</t>
+  </si>
+  <si>
+    <t>Physical activity</t>
+  </si>
+  <si>
+    <t>thinking about how to change routines that often lead to cravings to smoke</t>
+  </si>
+  <si>
+    <t>Thinking about how to change routines that often lead to cravings to smoke</t>
+  </si>
+  <si>
+    <t>think about how to change routines that often lead to cravings to smoke</t>
+  </si>
+  <si>
+    <t>AVOID smoking</t>
+  </si>
+  <si>
+    <t>may make it HARDER to refrain from smoking</t>
+  </si>
+  <si>
+    <t>get FEWER cravings to smoke</t>
+  </si>
+  <si>
+    <t>RESIST cravings to smoke</t>
+  </si>
+  <si>
+    <t>may make it DIFFICULT to refrain when you have a craving to smoke</t>
+  </si>
+  <si>
+    <t>prepare for and thus RESIST cravings to smoke</t>
+  </si>
+  <si>
+    <t>may make it HARD to prepare for and thus resist cravings to smoke</t>
+  </si>
+  <si>
+    <t>FOCUS on the goal of becoming more physically active</t>
+  </si>
+  <si>
+    <t>may cause you to LOOSE SIGHT of the goal of becoming more physically active</t>
+  </si>
+  <si>
+    <t>learning about the possible positive impact of physical activity on dealing with cravings to smoke</t>
+  </si>
+  <si>
+    <t>Learning about the possible positive impact of physical activity on dealing with cravings to smoke</t>
+  </si>
+  <si>
+    <t>learn about the possible positive impact of physical activity on dealing with cravings to smoke</t>
+  </si>
+  <si>
+    <t>feel more MOTIVATED to successfully quit smoking</t>
+  </si>
+  <si>
+    <t>thinking about the person you would like to be once you have successfully quit smoking</t>
+  </si>
+  <si>
+    <t>may lead to INSUFFICIENT motivation to successfully quit smoking</t>
+  </si>
+  <si>
+    <t>record your current physical activity routines</t>
+  </si>
+  <si>
+    <t>recording your current physical activity routines</t>
+  </si>
+  <si>
+    <t>Recording your current physical activity routines</t>
+  </si>
+  <si>
+    <t>record my current physical activity routines</t>
+  </si>
+  <si>
+    <t>Formulation Email</t>
+  </si>
+  <si>
+    <t>Formulation Chat</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, before the next session, please watch the following 2-minute video on how much and which type of physical activity is recommended: https://www.youtube.com/watch?v=AAPhWbG_zLs&amp;ab_channel=TREKGroup. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for this is to have high ambition to become more physically active. Thus, before the next session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, before the next session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Write down everything that comes to your mind. </t>
+  </si>
+  <si>
+    <t>It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, before the next session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Then, look for a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for this is to focus on the goal of becoming more physically active. Thus, before the next session, please take some time to visualize becoming more physically active as a battle. For example, you might see yourself and non-active version of yourself as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high motivation to become more physically active. Thus, before the next session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Then look for a picture that best captures your desired future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, before the next session, please think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, before the next session, please watch the following 5-minute video about the possible positive impact of physical activity on dealing with cravings to smoke: https://www.youtube.com/watch?v=StM10jzbt1k&amp;ab_channel=TreeHouseRecovery. What do you think about the information in the video? Write down your thoughts in a few words.</t>
+  </si>
+  <si>
+    <t>Being more physically active (e.g. exercise, take walks, spend less time sitting) may aid you to stop smoking. One important aspect for this is to have strong resolve to become more physically active. So, before the next session, please take some time to think of a personal rule that helps you to become more physically active. Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have a strong desire to become more physically active. Therefore, before the next session, please identify and write down reasons why you want to become more physically active. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for becoming more physically active is to remove possible obstacles. Thus, before the next session, please think about things that make it difficult for you to be physically active. For example, this could be that you do NOT have a raincoat to bike to the grocery store when it is raining, that you do NOT want to work out alone, or that you are at work all day and too exhausted by the time that you come home. What are possible solutions to your barriers? For instance, you could buy a raincoat, join a running group, or take a walk during your lunch break at work. Please write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may make it easier to successfully quit smoking. One important step for becoming more physically active is to know one's current level. This allows to later set a precise goal and hence to feel more motivated. So, please record your current behavior with regards to physical activity before the next session. Try to keep track of how much time you spend 1) sitting, 2) working out and 3) being moderately active (e.g. taking a walk, biking to the grocery store). For this, it might be helpful to keep a piece of paper and pen on your kitchen table, or maybe you have a smart watch that can record these types of behavior for you.</t>
+  </si>
+  <si>
+    <t>Preparing for situations in which you commonly smoke may make it easier to successfully quit smoking. Therefore, please record the situations in which you smoke before the next session. Take note of one or two keywords to describe the situation and the number of cigarettes that you smoked. For example, you might note "Lunch break, 2 cigarettes" or "TV, 5 cigarettes." It might be helpful to take these notes on your phone, or you could carry a small piece of paper and pen in your pocket.</t>
+  </si>
+  <si>
+    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, before the next session, please watch the following 12-minute video on how the body starts repairing itself immediately, as soon as a person stops smoking: https://www.youtube.com/watch?v=ZhTOC0T3P3c&amp;ab_channel=RespiratoryTherapyZone. What information from the video is most relevant to you? Take a few notes.</t>
+  </si>
+  <si>
+    <t>Having strong determination to refrain from smoking may help to quit successfully. So, before the next session, please take some time to think of a personal rule that helps you to refrain from smoking. Possible examples include "Not a puff - no matter what,” "Say no to smoking, yes to life" or "Smoking is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
+  </si>
+  <si>
+    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, before the next session, please watch the following 15-minute video to learn progressive muscle relaxation (which is a way of relaxing your body): https://www.youtube.com/watch?v=ihO02wUzgkc&amp;ab_channel=MarkConnelly. Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
+  </si>
+  <si>
+    <t>Planning how to resist urges to smoke may make it easier to successfully quit smoking. Therefore, before the next session, please think of activities that you could do to keep yourself busy when you feel the urge to smoke so that you do NOT smoke. These urges typically last a few minutes; think of something that you could do in the meantime until the urge has passed. For example, you could water your plants, eat a carrot, do 10 push-ups, or do something for another person in need. Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Preparing for situations in which avoiding to smoke is difficult may make it easier to successfully quit smoking. Thus, before the next session, please think about situations in which you might find it difficult to refrain from smoking. For example, this could be during your lunch break at work, when you meet your best friend, or when you watch TV. How could you deal with these situations so that you do NOT smoke? Write down your plans in a few words.</t>
+  </si>
+  <si>
+    <t>Getting fewer cravings to smoke may make it easier to successfully quit smoking. Therefore, before the next session, please think about routines in your daily life that often cause you to get cravings to smoke. For example, you might have experienced that if you go to bed very late and thus sleep less, you smoke more the next day. Or maybe you have noticed that if you skip your breakfast, you always smoke on your way to work but NOT otherwise. How could you change these routines to reduce or even avoid those cravings? Please write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Focusing on your goal of successfully quitting smoking may help to quit. Thus, before the next session, please take some time to visualize smoking as a battle. For example, you might see yourself and a cigarette as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
+  </si>
+  <si>
+    <t>Having high motivation to quit smoking may help to quit successfully. So, before the next session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Then, look for or take a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having high motivation to quit smoking may aid quitting successfully. Thus, before the next session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Write down everything that comes to your mind. </t>
+  </si>
+  <si>
+    <t>Having high aspiration to quit smoking may aid quitting successfully. So, before the next session, please identify and write down reasons why you want to stop smoking. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
+  </si>
+  <si>
+    <t>Having high aspiration to quit smoking may aid quitting successfully. Thus, before the next session, please think about the person that you would like to be once you have successfully quit smoking. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Having high aspiration to quit smoking may aid quitting successfully. Thus, *after* this session, please think about the person that you would like to be once you have successfully quit smoking. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Having high aspiration to quit smoking may aid quitting successfully. So, *after* this session, please identify and write down reasons why you want to stop smoking. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having high motivation to quit smoking may aid quitting successfully. Thus, *after* this session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Write down everything that comes to your mind. </t>
+  </si>
+  <si>
+    <t>Having high motivation to quit smoking may help to quit successfully. So, *after* this session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Then, look for or take a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Focusing on your goal of successfully quitting smoking may help to quit. Thus, *after* this session, please take some time to visualize smoking as a battle. For example, you might see yourself and a cigarette as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
+  </si>
+  <si>
+    <t>Getting fewer cravings to smoke may make it easier to successfully quit smoking. Therefore, *after* this session, please think about routines in your daily life that often cause you to get cravings to smoke. For example, you might have experienced that if you go to bed very late and thus sleep less, you smoke more the next day. Or maybe you have noticed that if you skip your breakfast, you always smoke on your way to work but NOT otherwise. How could you change these routines to reduce or even avoid those cravings? Please write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Preparing for situations in which avoiding to smoke is difficult may make it easier to successfully quit smoking. Thus, *after* this session, please think about situations in which you might find it difficult to refrain from smoking. For example, this could be during your lunch break at work, when you meet your best friend, or when you watch TV. How could you deal with these situations so that you do NOT smoke? Write down your plans in a few words.</t>
+  </si>
+  <si>
+    <t>Planning how to resist urges to smoke may make it easier to successfully quit smoking. Therefore, *after* this session, please think of activities that you could do to keep yourself busy when you feel the urge to smoke so that you do NOT smoke. These urges typically last a few minutes; think of something that you could do in the meantime until the urge has passed. For example, you could water your plants, eat a carrot, do 10 push-ups, or do something for another person in need. Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, *after* this session, please watch the 15-minute video that I will send you as a message in Prolific. The video will help you to learn progressive muscle relaxation (which is a way of relaxing your body). Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
+  </si>
+  <si>
+    <t>Having strong determination to refrain from smoking may help to quit successfully. So, *after* this session, please take some time to think of a personal rule that helps you to refrain from smoking. Possible examples include "Not a puff - no matter what,” "Say no to smoking, yes to life" or "Smoking is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
+  </si>
+  <si>
+    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, *after* this session, please watch the 12-minute video that I will send you as a message in Prolific. The video explains how the body starts repairing itself immediately, as soon as a person stops smoking. What information from the video is most relevant to you? Take a few notes.</t>
+  </si>
+  <si>
+    <t>Preparing for situations in which you commonly smoke may make it easier to successfully quit smoking. Therefore, please record the situations in which you smoke *after* this session. Take note of one or two keywords to describe the situation and the number of cigarettes that you smoked. For example, you might note "Lunch break, 2 cigarettes" or "TV, 5 cigarettes." It might be helpful to take these notes on your phone, or you could carry a small piece of paper and pen in your pocket.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may make it easier to successfully quit smoking. One important step for becoming more physically active is to know one's current level. This allows to later set a precise goal and hence to feel more motivated. So, please record your current behavior with regards to physical activity *after* this session. Try to keep track of how much time you spend 1) sitting, 2) working out and 3) being moderately active (e.g. taking a walk, biking to the grocery store). For this, it might be helpful to keep a piece of paper and pen on your kitchen table, or maybe you have a smart watch that can record these types of behavior for you.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for becoming more physically active is to remove possible obstacles. Thus, *after* this session, please think about things that make it difficult for you to be physically active. For example, this could be that you do NOT have a raincoat to bike to the grocery store when it is raining, that you do NOT want to work out alone, or that you are at work all day and too exhausted by the time that you come home. What are possible solutions to your barriers? For instance, you could buy a raincoat, join a running group, or take a walk during your lunch break at work. Please write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have a strong desire to become more physically active. Therefore, *after* this session, please identify and write down reasons why you want to become more physically active. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, *after* this session, please watch the 2-minute video that I will send you as a message in Prolific. The video explains how much and which type of physical activity is recommended. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for this is to have high ambition to become more physically active. Thus, *after* this session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, *after* this session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Write down everything that comes to your mind. </t>
+  </si>
+  <si>
+    <t>It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, *after* this session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Then, look for a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for this is to focus on the goal of becoming more physically active. Thus, *after* this session, please take some time to visualize becoming more physically active as a battle. For example, you might see yourself and non-active version of yourself as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high motivation to become more physically active. Thus, *after* this session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Then look for a picture that best captures your desired future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, *after* this session, please think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, *after* this session, please watch the 5-minute video that I will send you as a message in Prolific. The video explains the possible positive impact of physical activity on dealing with cravings to smoke. What do you think about the information in the video? Write down your thoughts in a few words.</t>
+  </si>
+  <si>
+    <t>Being more physically active (e.g. exercise, take walks, spend less time sitting) may aid you to stop smoking. One important aspect for this is to have strong resolve to become more physically active. So, *after* this session, please take some time to think of a personal rule that helps you to become more physically active. Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
+  </si>
+  <si>
+    <t>16,20</t>
+  </si>
+  <si>
+    <t>3,18,17</t>
+  </si>
+  <si>
+    <t>2,18,17</t>
+  </si>
+  <si>
+    <t>8,</t>
+  </si>
+  <si>
+    <t>22,</t>
+  </si>
+  <si>
+    <t>0, 20</t>
+  </si>
+  <si>
+    <t>18,2,3</t>
+  </si>
+  <si>
+    <t>17,3,2</t>
+  </si>
+  <si>
+    <t>0,16</t>
+  </si>
+  <si>
+    <t>15,</t>
+  </si>
+  <si>
     <t>9,</t>
-  </si>
-  <si>
-    <t>recording your current smoking behavior</t>
-  </si>
-  <si>
-    <t>Recording your current smoking behavior</t>
-  </si>
-  <si>
-    <t>record your current smoking behavior</t>
-  </si>
-  <si>
-    <t>record my current smoking behavior</t>
-  </si>
-  <si>
-    <t>None, but helps for the activities that ask to come up with routines etc.</t>
-  </si>
-  <si>
-    <t>PA</t>
-  </si>
-  <si>
-    <t>become more physically active</t>
-  </si>
-  <si>
-    <t>thinking about solutions to possible barriers</t>
-  </si>
-  <si>
-    <t>thinking about solutions to barriers</t>
-  </si>
-  <si>
-    <t>Thinking about solutions to barriers</t>
-  </si>
-  <si>
-    <t>think about solutions to barriers</t>
-  </si>
-  <si>
-    <t>Thinking about solutions to possible barriers</t>
-  </si>
-  <si>
-    <t>think about solutions to possible barriers</t>
-  </si>
-  <si>
-    <t>REMOVE obstacles to becoming more physically active</t>
-  </si>
-  <si>
-    <t>may cause those barriers to PREVENT you from becoming more physically active</t>
-  </si>
-  <si>
-    <t>identifying reasons why you want to become more physically active</t>
-  </si>
-  <si>
-    <t>Identifying reasons why you want to become more physically active</t>
-  </si>
-  <si>
-    <t>identify reasons why you want to become more physically active</t>
-  </si>
-  <si>
-    <t>identify reasons why I want to become more physically active</t>
-  </si>
-  <si>
-    <t>increase your DESIRE to become more physically active</t>
-  </si>
-  <si>
-    <t>may lead to a LACK of desire to become more physically active</t>
-  </si>
-  <si>
-    <t>comparing your current physical activity behavior to what is recommended</t>
-  </si>
-  <si>
-    <t>comparing your physical activity behavior to what is recommended</t>
-  </si>
-  <si>
-    <t>Comparing your physical activity behavior to what is recommended</t>
-  </si>
-  <si>
-    <t>compare your physical activity behavior to what is recommended</t>
-  </si>
-  <si>
-    <t>compare my physical activity behavior to what is recommended</t>
-  </si>
-  <si>
-    <t>Comparing your current physical activity behavior to what is recommended</t>
-  </si>
-  <si>
-    <t>compare your current physical activity behavior to what is recommended</t>
-  </si>
-  <si>
-    <t>compare my current physical activity behavior to what is recommended</t>
-  </si>
-  <si>
-    <t>13,</t>
-  </si>
-  <si>
-    <t>23,</t>
-  </si>
-  <si>
-    <t>thinking about the person you would like to be once you have become more physically active</t>
-  </si>
-  <si>
-    <t>Thinking about the person you would like to be once you have become more physically active</t>
-  </si>
-  <si>
-    <t>think about the person you would like to be once you have become more physically active</t>
-  </si>
-  <si>
-    <t>think about the person I would like to be once I have become more physically active</t>
-  </si>
-  <si>
-    <t>increase your AMBITION to become a more physically active person</t>
-  </si>
-  <si>
-    <t>may lead to a LACK of ambition to become a more physically active person</t>
-  </si>
-  <si>
-    <t>1, 21</t>
-  </si>
-  <si>
-    <t>thinking about who you do NOT want to be but might become if you fail to become more physically active</t>
-  </si>
-  <si>
-    <t>Thinking about who you do NOT want to be but might become if you fail to become more physically active</t>
-  </si>
-  <si>
-    <t>think about who you do NOT want to be but might become if you fail to become more physically active</t>
-  </si>
-  <si>
-    <t>think about who I do NOT want to be but might become if I fail to become more physically active</t>
-  </si>
-  <si>
-    <t>heighten your DETERMINATION to become a more physically active person</t>
-  </si>
-  <si>
-    <t>may lead to INSUFFICIENT determination to become a more physically active person</t>
-  </si>
-  <si>
-    <t>19,3,4</t>
-  </si>
-  <si>
-    <t>18,4,3</t>
-  </si>
-  <si>
-    <t>visualizing becoming more physically active as a battle that you win</t>
-  </si>
-  <si>
-    <t>Visualizing becoming more physically active as a battle that you win</t>
-  </si>
-  <si>
-    <t>visualize becoming more physically active as a battle that you win</t>
-  </si>
-  <si>
-    <t>visualize becoming more physically active as a battle that I win</t>
-  </si>
-  <si>
-    <t>feel more MOTIVATED to become a more physically active person</t>
-  </si>
-  <si>
-    <t>may lead to INSUFFICIENT motivation to become a more physically active person</t>
-  </si>
-  <si>
-    <t>1,17</t>
-  </si>
-  <si>
-    <t>thinking about what you could do to become more physically active</t>
-  </si>
-  <si>
-    <t>Thinking about what you could do to become more physically active</t>
-  </si>
-  <si>
-    <t>think about what you could do to become more physically active</t>
-  </si>
-  <si>
-    <t>think about what I could do to become more physically active</t>
-  </si>
-  <si>
-    <t>SUCCEED at becoming more physically active</t>
-  </si>
-  <si>
-    <t>may make it DIFFICULT to become more physically active</t>
-  </si>
-  <si>
-    <t>heighten your ASPIRATION to become more physically active</t>
-  </si>
-  <si>
-    <t>may lead to a LACK of aspiration to become more physically active</t>
-  </si>
-  <si>
-    <t>16,</t>
-  </si>
-  <si>
-    <t>generate strong RESOLVE to become more physically active</t>
-  </si>
-  <si>
-    <t>may lead to INSUFFICIENT resolve to become more physically active</t>
-  </si>
-  <si>
-    <t>10,</t>
-  </si>
-  <si>
-    <t>set a SPECIFIC GOAL and thus to feel more ASPIRATION to become more physically active</t>
-  </si>
-  <si>
-    <t>set a PRECISE GOAL and thus to feel more MOTIVATED to become more physically active</t>
-  </si>
-  <si>
-    <t>may make it DIFFICULT to set a precise goal and thus lead to INSUFFICIENT motivation to become more physically active</t>
-  </si>
-  <si>
-    <t>may make it HARD to set a specific goal and thus lead to INSUFFICIENT aspiration to become more physically active</t>
-  </si>
-  <si>
-    <t>Experts</t>
-  </si>
-  <si>
-    <t>Smoking cessation</t>
-  </si>
-  <si>
-    <t>Physical activity</t>
-  </si>
-  <si>
-    <t>thinking about how to change routines that often lead to cravings to smoke</t>
-  </si>
-  <si>
-    <t>Thinking about how to change routines that often lead to cravings to smoke</t>
-  </si>
-  <si>
-    <t>think about how to change routines that often lead to cravings to smoke</t>
-  </si>
-  <si>
-    <t>AVOID smoking</t>
-  </si>
-  <si>
-    <t>may make it HARDER to refrain from smoking</t>
-  </si>
-  <si>
-    <t>get FEWER cravings to smoke</t>
-  </si>
-  <si>
-    <t>RESIST cravings to smoke</t>
-  </si>
-  <si>
-    <t>may make it DIFFICULT to refrain when you have a craving to smoke</t>
-  </si>
-  <si>
-    <t>prepare for and thus RESIST cravings to smoke</t>
-  </si>
-  <si>
-    <t>may make it HARD to prepare for and thus resist cravings to smoke</t>
-  </si>
-  <si>
-    <t>FOCUS on the goal of becoming more physically active</t>
-  </si>
-  <si>
-    <t>may cause you to LOOSE SIGHT of the goal of becoming more physically active</t>
-  </si>
-  <si>
-    <t>learning about the possible positive impact of physical activity on dealing with cravings to smoke</t>
-  </si>
-  <si>
-    <t>Learning about the possible positive impact of physical activity on dealing with cravings to smoke</t>
-  </si>
-  <si>
-    <t>learn about the possible positive impact of physical activity on dealing with cravings to smoke</t>
-  </si>
-  <si>
-    <t>feel more MOTIVATED to successfully quit smoking</t>
-  </si>
-  <si>
-    <t>thinking about the person you would like to be once you have successfully quit smoking</t>
-  </si>
-  <si>
-    <t>may lead to INSUFFICIENT motivation to successfully quit smoking</t>
-  </si>
-  <si>
-    <t>record your current physical activity routines</t>
-  </si>
-  <si>
-    <t>recording your current physical activity routines</t>
-  </si>
-  <si>
-    <t>Recording your current physical activity routines</t>
-  </si>
-  <si>
-    <t>record my current physical activity routines</t>
-  </si>
-  <si>
-    <t>Formulation Email</t>
-  </si>
-  <si>
-    <t>Formulation Chat</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, before the next session, please watch the following 2-minute video on how much and which type of physical activity is recommended: https://www.youtube.com/watch?v=AAPhWbG_zLs&amp;ab_channel=TREKGroup. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for this is to have high ambition to become more physically active. Thus, before the next session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, before the next session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Write down everything that comes to your mind. </t>
-  </si>
-  <si>
-    <t>It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, before the next session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Then, look for a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for this is to focus on the goal of becoming more physically active. Thus, before the next session, please take some time to visualize becoming more physically active as a battle. For example, you might see yourself and non-active version of yourself as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high motivation to become more physically active. Thus, before the next session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Then look for a picture that best captures your desired future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, before the next session, please think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, before the next session, please watch the following 5-minute video about the possible positive impact of physical activity on dealing with cravings to smoke: https://www.youtube.com/watch?v=StM10jzbt1k&amp;ab_channel=TreeHouseRecovery. What do you think about the information in the video? Write down your thoughts in a few words.</t>
-  </si>
-  <si>
-    <t>Being more physically active (e.g. exercise, take walks, spend less time sitting) may aid you to stop smoking. One important aspect for this is to have strong resolve to become more physically active. So, before the next session, please take some time to think of a personal rule that helps you to become more physically active. Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have a strong desire to become more physically active. Therefore, before the next session, please identify and write down reasons why you want to become more physically active. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for becoming more physically active is to remove possible obstacles. Thus, before the next session, please think about things that make it difficult for you to be physically active. For example, this could be that you do NOT have a raincoat to bike to the grocery store when it is raining, that you do NOT want to work out alone, or that you are at work all day and too exhausted by the time that you come home. What are possible solutions to your barriers? For instance, you could buy a raincoat, join a running group, or take a walk during your lunch break at work. Please write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may make it easier to successfully quit smoking. One important step for becoming more physically active is to know one's current level. This allows to later set a precise goal and hence to feel more motivated. So, please record your current behavior with regards to physical activity before the next session. Try to keep track of how much time you spend 1) sitting, 2) working out and 3) being moderately active (e.g. taking a walk, biking to the grocery store). For this, it might be helpful to keep a piece of paper and pen on your kitchen table, or maybe you have a smart watch that can record these types of behavior for you.</t>
-  </si>
-  <si>
-    <t>Preparing for situations in which you commonly smoke may make it easier to successfully quit smoking. Therefore, please record the situations in which you smoke before the next session. Take note of one or two keywords to describe the situation and the number of cigarettes that you smoked. For example, you might note "Lunch break, 2 cigarettes" or "TV, 5 cigarettes." It might be helpful to take these notes on your phone, or you could carry a small piece of paper and pen in your pocket.</t>
-  </si>
-  <si>
-    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, before the next session, please watch the following 12-minute video on how the body starts repairing itself immediately, as soon as a person stops smoking: https://www.youtube.com/watch?v=ZhTOC0T3P3c&amp;ab_channel=RespiratoryTherapyZone. What information from the video is most relevant to you? Take a few notes.</t>
-  </si>
-  <si>
-    <t>Having strong determination to refrain from smoking may help to quit successfully. So, before the next session, please take some time to think of a personal rule that helps you to refrain from smoking. Possible examples include "Not a puff - no matter what,” "Say no to smoking, yes to life" or "Smoking is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
-  </si>
-  <si>
-    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, before the next session, please watch the following 15-minute video to learn progressive muscle relaxation (which is a way of relaxing your body): https://www.youtube.com/watch?v=ihO02wUzgkc&amp;ab_channel=MarkConnelly. Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
-  </si>
-  <si>
-    <t>Planning how to resist urges to smoke may make it easier to successfully quit smoking. Therefore, before the next session, please think of activities that you could do to keep yourself busy when you feel the urge to smoke so that you do NOT smoke. These urges typically last a few minutes; think of something that you could do in the meantime until the urge has passed. For example, you could water your plants, eat a carrot, do 10 push-ups, or do something for another person in need. Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Preparing for situations in which avoiding to smoke is difficult may make it easier to successfully quit smoking. Thus, before the next session, please think about situations in which you might find it difficult to refrain from smoking. For example, this could be during your lunch break at work, when you meet your best friend, or when you watch TV. How could you deal with these situations so that you do NOT smoke? Write down your plans in a few words.</t>
-  </si>
-  <si>
-    <t>Getting fewer cravings to smoke may make it easier to successfully quit smoking. Therefore, before the next session, please think about routines in your daily life that often cause you to get cravings to smoke. For example, you might have experienced that if you go to bed very late and thus sleep less, you smoke more the next day. Or maybe you have noticed that if you skip your breakfast, you always smoke on your way to work but NOT otherwise. How could you change these routines to reduce or even avoid those cravings? Please write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Focusing on your goal of successfully quitting smoking may help to quit. Thus, before the next session, please take some time to visualize smoking as a battle. For example, you might see yourself and a cigarette as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
-  </si>
-  <si>
-    <t>Having high motivation to quit smoking may help to quit successfully. So, before the next session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Then, look for or take a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Having high motivation to quit smoking may aid quitting successfully. Thus, before the next session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Write down everything that comes to your mind. </t>
-  </si>
-  <si>
-    <t>Having high aspiration to quit smoking may aid quitting successfully. So, before the next session, please identify and write down reasons why you want to stop smoking. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
-  </si>
-  <si>
-    <t>Having high aspiration to quit smoking may aid quitting successfully. Thus, before the next session, please think about the person that you would like to be once you have successfully quit smoking. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Having high aspiration to quit smoking may aid quitting successfully. Thus, *after* this session, please think about the person that you would like to be once you have successfully quit smoking. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Having high aspiration to quit smoking may aid quitting successfully. So, *after* this session, please identify and write down reasons why you want to stop smoking. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Having high motivation to quit smoking may aid quitting successfully. Thus, *after* this session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Write down everything that comes to your mind. </t>
-  </si>
-  <si>
-    <t>Having high motivation to quit smoking may help to quit successfully. So, *after* this session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Then, look for or take a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t>Focusing on your goal of successfully quitting smoking may help to quit. Thus, *after* this session, please take some time to visualize smoking as a battle. For example, you might see yourself and a cigarette as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
-  </si>
-  <si>
-    <t>Getting fewer cravings to smoke may make it easier to successfully quit smoking. Therefore, *after* this session, please think about routines in your daily life that often cause you to get cravings to smoke. For example, you might have experienced that if you go to bed very late and thus sleep less, you smoke more the next day. Or maybe you have noticed that if you skip your breakfast, you always smoke on your way to work but NOT otherwise. How could you change these routines to reduce or even avoid those cravings? Please write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Preparing for situations in which avoiding to smoke is difficult may make it easier to successfully quit smoking. Thus, *after* this session, please think about situations in which you might find it difficult to refrain from smoking. For example, this could be during your lunch break at work, when you meet your best friend, or when you watch TV. How could you deal with these situations so that you do NOT smoke? Write down your plans in a few words.</t>
-  </si>
-  <si>
-    <t>Planning how to resist urges to smoke may make it easier to successfully quit smoking. Therefore, *after* this session, please think of activities that you could do to keep yourself busy when you feel the urge to smoke so that you do NOT smoke. These urges typically last a few minutes; think of something that you could do in the meantime until the urge has passed. For example, you could water your plants, eat a carrot, do 10 push-ups, or do something for another person in need. Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, *after* this session, please watch the 15-minute video that I will send you as a message in Prolific. The video will help you to learn progressive muscle relaxation (which is a way of relaxing your body). Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
-  </si>
-  <si>
-    <t>Having strong determination to refrain from smoking may help to quit successfully. So, *after* this session, please take some time to think of a personal rule that helps you to refrain from smoking. Possible examples include "Not a puff - no matter what,” "Say no to smoking, yes to life" or "Smoking is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
-  </si>
-  <si>
-    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, *after* this session, please watch the 12-minute video that I will send you as a message in Prolific. The video explains how the body starts repairing itself immediately, as soon as a person stops smoking. What information from the video is most relevant to you? Take a few notes.</t>
-  </si>
-  <si>
-    <t>Preparing for situations in which you commonly smoke may make it easier to successfully quit smoking. Therefore, please record the situations in which you smoke *after* this session. Take note of one or two keywords to describe the situation and the number of cigarettes that you smoked. For example, you might note "Lunch break, 2 cigarettes" or "TV, 5 cigarettes." It might be helpful to take these notes on your phone, or you could carry a small piece of paper and pen in your pocket.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may make it easier to successfully quit smoking. One important step for becoming more physically active is to know one's current level. This allows to later set a precise goal and hence to feel more motivated. So, please record your current behavior with regards to physical activity *after* this session. Try to keep track of how much time you spend 1) sitting, 2) working out and 3) being moderately active (e.g. taking a walk, biking to the grocery store). For this, it might be helpful to keep a piece of paper and pen on your kitchen table, or maybe you have a smart watch that can record these types of behavior for you.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for becoming more physically active is to remove possible obstacles. Thus, *after* this session, please think about things that make it difficult for you to be physically active. For example, this could be that you do NOT have a raincoat to bike to the grocery store when it is raining, that you do NOT want to work out alone, or that you are at work all day and too exhausted by the time that you come home. What are possible solutions to your barriers? For instance, you could buy a raincoat, join a running group, or take a walk during your lunch break at work. Please write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have a strong desire to become more physically active. Therefore, *after* this session, please identify and write down reasons why you want to become more physically active. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, *after* this session, please watch the 2-minute video that I will send you as a message in Prolific. The video explains how much and which type of physical activity is recommended. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for this is to have high ambition to become more physically active. Thus, *after* this session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, *after* this session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Write down everything that comes to your mind. </t>
-  </si>
-  <si>
-    <t>It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, *after* this session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Then, look for a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for this is to focus on the goal of becoming more physically active. Thus, *after* this session, please take some time to visualize becoming more physically active as a battle. For example, you might see yourself and non-active version of yourself as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high motivation to become more physically active. Thus, *after* this session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Then look for a picture that best captures your desired future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, *after* this session, please think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, *after* this session, please watch the 5-minute video that I will send you as a message in Prolific. The video explains the possible positive impact of physical activity on dealing with cravings to smoke. What do you think about the information in the video? Write down your thoughts in a few words.</t>
-  </si>
-  <si>
-    <t>Being more physically active (e.g. exercise, take walks, spend less time sitting) may aid you to stop smoking. One important aspect for this is to have strong resolve to become more physically active. So, *after* this session, please take some time to think of a personal rule that helps you to become more physically active. Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
   </si>
 </sst>
 </file>
@@ -1561,8 +1561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1580,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1622,16 +1622,16 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1639,10 +1639,10 @@
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>17</v>
@@ -1676,16 +1676,16 @@
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="115.2" x14ac:dyDescent="0.3">
@@ -1696,51 +1696,51 @@
         <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
@@ -1751,53 +1751,53 @@
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="L4" s="1" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>44</v>
+        <v>222</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="216" x14ac:dyDescent="0.3">
@@ -1808,56 +1808,56 @@
         <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="L5" s="1" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>45</v>
+        <v>223</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1865,51 +1865,51 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="I6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="M6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="230.4" x14ac:dyDescent="0.3">
@@ -1920,53 +1920,53 @@
         <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
@@ -1977,53 +1977,53 @@
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="H8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I8" s="1" t="s">
+      <c r="L8" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="O8" s="1" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="216" x14ac:dyDescent="0.3">
@@ -2034,51 +2034,51 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="L9" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
@@ -2089,53 +2089,53 @@
         <v>16</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="I10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="L10" s="1" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
-        <v>70</v>
+        <v>141</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
@@ -2146,53 +2146,53 @@
         <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="M11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="172.8" x14ac:dyDescent="0.3">
@@ -2203,56 +2203,56 @@
         <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="L12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="M12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>87</v>
+        <v>224</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2260,51 +2260,51 @@
         <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -2312,105 +2312,105 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="302.39999999999998" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="288" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="H15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="K15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L15" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="172.8" x14ac:dyDescent="0.3">
@@ -2418,54 +2418,54 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -2473,56 +2473,56 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="L17" s="1" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>118</v>
+        <v>225</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="230.4" x14ac:dyDescent="0.3">
@@ -2530,13 +2530,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>17</v>
@@ -2551,33 +2551,33 @@
         <v>20</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="M18" s="1"/>
       <c r="N18" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1" t="s">
-        <v>125</v>
+        <v>226</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="259.2" x14ac:dyDescent="0.3">
@@ -2585,54 +2585,54 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="I19" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1" t="s">
-        <v>132</v>
+        <v>227</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="288" x14ac:dyDescent="0.3">
@@ -2640,54 +2640,54 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="I20" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="M20" s="1"/>
       <c r="N20" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1" t="s">
-        <v>133</v>
+        <v>228</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="230.4" x14ac:dyDescent="0.3">
@@ -2695,52 +2695,52 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="M21" s="1"/>
       <c r="N21" s="1" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="259.2" x14ac:dyDescent="0.3">
@@ -2748,13 +2748,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>17</v>
@@ -2769,86 +2769,86 @@
         <v>20</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="M22" s="1"/>
       <c r="N22" s="1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1" t="s">
-        <v>140</v>
+        <v>229</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="230.4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="216" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="230.4" x14ac:dyDescent="0.3">
@@ -2856,54 +2856,54 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1" t="s">
-        <v>149</v>
+        <v>230</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="244.8" x14ac:dyDescent="0.3">
@@ -2911,54 +2911,54 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="M25" s="1"/>
       <c r="N25" s="1" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1" t="s">
-        <v>152</v>
+        <v>231</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exclusion for 2 battle activities added
</commit_message>
<xml_diff>
--- a/Activities.xlsx
+++ b/Activities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\CAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A2870F-8481-4A97-B768-0D0C6DFEA2C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DE128D-E93E-41AA-859E-B5415081F6E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="234">
   <si>
     <t>Number</t>
   </si>
@@ -716,6 +716,12 @@
   </si>
   <si>
     <t>9,</t>
+  </si>
+  <si>
+    <t>4,</t>
+  </si>
+  <si>
+    <t>19,</t>
   </si>
 </sst>
 </file>
@@ -1561,8 +1567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1901,7 +1907,9 @@
         <v>48</v>
       </c>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1" t="s">
+        <v>233</v>
+      </c>
       <c r="Q6" s="1" t="s">
         <v>201</v>
       </c>
@@ -2732,7 +2740,9 @@
         <v>160</v>
       </c>
       <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
+      <c r="P21" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="Q21" s="1" t="s">
         <v>216</v>
       </c>

</xml_diff>

<commit_message>
advise rather than ask to do activities in activity formulations
</commit_message>
<xml_diff>
--- a/Activities.xlsx
+++ b/Activities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DE128D-E93E-41AA-859E-B5415081F6E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF5CC9D-42EB-4446-934F-99ADCBB3826C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -541,150 +541,6 @@
     <t>Formulation Chat</t>
   </si>
   <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, before the next session, please watch the following 2-minute video on how much and which type of physical activity is recommended: https://www.youtube.com/watch?v=AAPhWbG_zLs&amp;ab_channel=TREKGroup. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for this is to have high ambition to become more physically active. Thus, before the next session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, before the next session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Write down everything that comes to your mind. </t>
-  </si>
-  <si>
-    <t>It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, before the next session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Then, look for a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for this is to focus on the goal of becoming more physically active. Thus, before the next session, please take some time to visualize becoming more physically active as a battle. For example, you might see yourself and non-active version of yourself as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high motivation to become more physically active. Thus, before the next session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Then look for a picture that best captures your desired future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, before the next session, please think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, before the next session, please watch the following 5-minute video about the possible positive impact of physical activity on dealing with cravings to smoke: https://www.youtube.com/watch?v=StM10jzbt1k&amp;ab_channel=TreeHouseRecovery. What do you think about the information in the video? Write down your thoughts in a few words.</t>
-  </si>
-  <si>
-    <t>Being more physically active (e.g. exercise, take walks, spend less time sitting) may aid you to stop smoking. One important aspect for this is to have strong resolve to become more physically active. So, before the next session, please take some time to think of a personal rule that helps you to become more physically active. Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have a strong desire to become more physically active. Therefore, before the next session, please identify and write down reasons why you want to become more physically active. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for becoming more physically active is to remove possible obstacles. Thus, before the next session, please think about things that make it difficult for you to be physically active. For example, this could be that you do NOT have a raincoat to bike to the grocery store when it is raining, that you do NOT want to work out alone, or that you are at work all day and too exhausted by the time that you come home. What are possible solutions to your barriers? For instance, you could buy a raincoat, join a running group, or take a walk during your lunch break at work. Please write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may make it easier to successfully quit smoking. One important step for becoming more physically active is to know one's current level. This allows to later set a precise goal and hence to feel more motivated. So, please record your current behavior with regards to physical activity before the next session. Try to keep track of how much time you spend 1) sitting, 2) working out and 3) being moderately active (e.g. taking a walk, biking to the grocery store). For this, it might be helpful to keep a piece of paper and pen on your kitchen table, or maybe you have a smart watch that can record these types of behavior for you.</t>
-  </si>
-  <si>
-    <t>Preparing for situations in which you commonly smoke may make it easier to successfully quit smoking. Therefore, please record the situations in which you smoke before the next session. Take note of one or two keywords to describe the situation and the number of cigarettes that you smoked. For example, you might note "Lunch break, 2 cigarettes" or "TV, 5 cigarettes." It might be helpful to take these notes on your phone, or you could carry a small piece of paper and pen in your pocket.</t>
-  </si>
-  <si>
-    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, before the next session, please watch the following 12-minute video on how the body starts repairing itself immediately, as soon as a person stops smoking: https://www.youtube.com/watch?v=ZhTOC0T3P3c&amp;ab_channel=RespiratoryTherapyZone. What information from the video is most relevant to you? Take a few notes.</t>
-  </si>
-  <si>
-    <t>Having strong determination to refrain from smoking may help to quit successfully. So, before the next session, please take some time to think of a personal rule that helps you to refrain from smoking. Possible examples include "Not a puff - no matter what,” "Say no to smoking, yes to life" or "Smoking is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
-  </si>
-  <si>
-    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, before the next session, please watch the following 15-minute video to learn progressive muscle relaxation (which is a way of relaxing your body): https://www.youtube.com/watch?v=ihO02wUzgkc&amp;ab_channel=MarkConnelly. Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
-  </si>
-  <si>
-    <t>Planning how to resist urges to smoke may make it easier to successfully quit smoking. Therefore, before the next session, please think of activities that you could do to keep yourself busy when you feel the urge to smoke so that you do NOT smoke. These urges typically last a few minutes; think of something that you could do in the meantime until the urge has passed. For example, you could water your plants, eat a carrot, do 10 push-ups, or do something for another person in need. Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Preparing for situations in which avoiding to smoke is difficult may make it easier to successfully quit smoking. Thus, before the next session, please think about situations in which you might find it difficult to refrain from smoking. For example, this could be during your lunch break at work, when you meet your best friend, or when you watch TV. How could you deal with these situations so that you do NOT smoke? Write down your plans in a few words.</t>
-  </si>
-  <si>
-    <t>Getting fewer cravings to smoke may make it easier to successfully quit smoking. Therefore, before the next session, please think about routines in your daily life that often cause you to get cravings to smoke. For example, you might have experienced that if you go to bed very late and thus sleep less, you smoke more the next day. Or maybe you have noticed that if you skip your breakfast, you always smoke on your way to work but NOT otherwise. How could you change these routines to reduce or even avoid those cravings? Please write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Focusing on your goal of successfully quitting smoking may help to quit. Thus, before the next session, please take some time to visualize smoking as a battle. For example, you might see yourself and a cigarette as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
-  </si>
-  <si>
-    <t>Having high motivation to quit smoking may help to quit successfully. So, before the next session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Then, look for or take a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Having high motivation to quit smoking may aid quitting successfully. Thus, before the next session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Write down everything that comes to your mind. </t>
-  </si>
-  <si>
-    <t>Having high aspiration to quit smoking may aid quitting successfully. So, before the next session, please identify and write down reasons why you want to stop smoking. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
-  </si>
-  <si>
-    <t>Having high aspiration to quit smoking may aid quitting successfully. Thus, before the next session, please think about the person that you would like to be once you have successfully quit smoking. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Having high aspiration to quit smoking may aid quitting successfully. Thus, *after* this session, please think about the person that you would like to be once you have successfully quit smoking. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Having high aspiration to quit smoking may aid quitting successfully. So, *after* this session, please identify and write down reasons why you want to stop smoking. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Having high motivation to quit smoking may aid quitting successfully. Thus, *after* this session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Write down everything that comes to your mind. </t>
-  </si>
-  <si>
-    <t>Having high motivation to quit smoking may help to quit successfully. So, *after* this session, please think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Then, look for or take a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t>Focusing on your goal of successfully quitting smoking may help to quit. Thus, *after* this session, please take some time to visualize smoking as a battle. For example, you might see yourself and a cigarette as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
-  </si>
-  <si>
-    <t>Getting fewer cravings to smoke may make it easier to successfully quit smoking. Therefore, *after* this session, please think about routines in your daily life that often cause you to get cravings to smoke. For example, you might have experienced that if you go to bed very late and thus sleep less, you smoke more the next day. Or maybe you have noticed that if you skip your breakfast, you always smoke on your way to work but NOT otherwise. How could you change these routines to reduce or even avoid those cravings? Please write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Preparing for situations in which avoiding to smoke is difficult may make it easier to successfully quit smoking. Thus, *after* this session, please think about situations in which you might find it difficult to refrain from smoking. For example, this could be during your lunch break at work, when you meet your best friend, or when you watch TV. How could you deal with these situations so that you do NOT smoke? Write down your plans in a few words.</t>
-  </si>
-  <si>
-    <t>Planning how to resist urges to smoke may make it easier to successfully quit smoking. Therefore, *after* this session, please think of activities that you could do to keep yourself busy when you feel the urge to smoke so that you do NOT smoke. These urges typically last a few minutes; think of something that you could do in the meantime until the urge has passed. For example, you could water your plants, eat a carrot, do 10 push-ups, or do something for another person in need. Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, *after* this session, please watch the 15-minute video that I will send you as a message in Prolific. The video will help you to learn progressive muscle relaxation (which is a way of relaxing your body). Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
-  </si>
-  <si>
-    <t>Having strong determination to refrain from smoking may help to quit successfully. So, *after* this session, please take some time to think of a personal rule that helps you to refrain from smoking. Possible examples include "Not a puff - no matter what,” "Say no to smoking, yes to life" or "Smoking is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
-  </si>
-  <si>
-    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, *after* this session, please watch the 12-minute video that I will send you as a message in Prolific. The video explains how the body starts repairing itself immediately, as soon as a person stops smoking. What information from the video is most relevant to you? Take a few notes.</t>
-  </si>
-  <si>
-    <t>Preparing for situations in which you commonly smoke may make it easier to successfully quit smoking. Therefore, please record the situations in which you smoke *after* this session. Take note of one or two keywords to describe the situation and the number of cigarettes that you smoked. For example, you might note "Lunch break, 2 cigarettes" or "TV, 5 cigarettes." It might be helpful to take these notes on your phone, or you could carry a small piece of paper and pen in your pocket.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may make it easier to successfully quit smoking. One important step for becoming more physically active is to know one's current level. This allows to later set a precise goal and hence to feel more motivated. So, please record your current behavior with regards to physical activity *after* this session. Try to keep track of how much time you spend 1) sitting, 2) working out and 3) being moderately active (e.g. taking a walk, biking to the grocery store). For this, it might be helpful to keep a piece of paper and pen on your kitchen table, or maybe you have a smart watch that can record these types of behavior for you.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for becoming more physically active is to remove possible obstacles. Thus, *after* this session, please think about things that make it difficult for you to be physically active. For example, this could be that you do NOT have a raincoat to bike to the grocery store when it is raining, that you do NOT want to work out alone, or that you are at work all day and too exhausted by the time that you come home. What are possible solutions to your barriers? For instance, you could buy a raincoat, join a running group, or take a walk during your lunch break at work. Please write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have a strong desire to become more physically active. Therefore, *after* this session, please identify and write down reasons why you want to become more physically active. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, *after* this session, please watch the 2-minute video that I will send you as a message in Prolific. The video explains how much and which type of physical activity is recommended. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for this is to have high ambition to become more physically active. Thus, *after* this session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, *after* this session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Write down everything that comes to your mind. </t>
-  </si>
-  <si>
-    <t>It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, *after* this session, please think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Then, look for a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for this is to focus on the goal of becoming more physically active. Thus, *after* this session, please take some time to visualize becoming more physically active as a battle. For example, you might see yourself and non-active version of yourself as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
-  </si>
-  <si>
-    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high motivation to become more physically active. Thus, *after* this session, please think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Then look for a picture that best captures your desired future self. Save or print this picture so that you can see it every day.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, *after* this session, please think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
-  </si>
-  <si>
-    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, *after* this session, please watch the 5-minute video that I will send you as a message in Prolific. The video explains the possible positive impact of physical activity on dealing with cravings to smoke. What do you think about the information in the video? Write down your thoughts in a few words.</t>
-  </si>
-  <si>
-    <t>Being more physically active (e.g. exercise, take walks, spend less time sitting) may aid you to stop smoking. One important aspect for this is to have strong resolve to become more physically active. So, *after* this session, please take some time to think of a personal rule that helps you to become more physically active. Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
-  </si>
-  <si>
     <t>16,20</t>
   </si>
   <si>
@@ -722,6 +578,150 @@
   </si>
   <si>
     <t>19,</t>
+  </si>
+  <si>
+    <t>Having high aspiration to quit smoking may aid quitting successfully. Thus, *after* this session, I recommend you to think about the person that you would like to be once you have successfully quit smoking. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Having high aspiration to quit smoking may aid quitting successfully. So, *after* this session, I advise you to identify and write down reasons why you want to stop smoking. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having high motivation to quit smoking may aid quitting successfully. Thus, *after* this session, I advise you to think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Write down everything that comes to your mind. </t>
+  </si>
+  <si>
+    <t>Having high motivation to quit smoking may help to quit successfully. So, *after* this session, I advise you to think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Then, look for or take a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Focusing on your goal of successfully quitting smoking may help to quit. Thus, *after* this session, I advise you to take some time to visualize smoking as a battle. For example, you might see yourself and a cigarette as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
+  </si>
+  <si>
+    <t>Getting fewer cravings to smoke may make it easier to successfully quit smoking. Therefore, *after* this session, I advise you to think about routines in your daily life that often cause you to get cravings to smoke. For example, you might have experienced that if you go to bed very late and thus sleep less, you smoke more the next day. Or maybe you have noticed that if you skip your breakfast, you always smoke on your way to work but NOT otherwise. How could you change these routines to reduce or even avoid those cravings? Please write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Preparing for situations in which avoiding to smoke is difficult may make it easier to successfully quit smoking. Thus, *after* this session, I advise you to think about situations in which you might find it difficult to refrain from smoking. For example, this could be during your lunch break at work, when you meet your best friend, or when you watch TV. How could you deal with these situations so that you do NOT smoke? Write down your plans in a few words.</t>
+  </si>
+  <si>
+    <t>Planning how to resist urges to smoke may make it easier to successfully quit smoking. Therefore, *after* this session, I advise you to think of activities that you could do to keep yourself busy when you feel the urge to smoke so that you do NOT smoke. These urges typically last a few minutes; think of something that you could do in the meantime until the urge has passed. For example, you could water your plants, eat a carrot, do 10 push-ups, or do something for another person in need. Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, *after* this session, I advise you to watch the 15-minute video that I will send you as a message in Prolific. The video will help you to learn progressive muscle relaxation (which is a way of relaxing your body). Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
+  </si>
+  <si>
+    <t>Having strong determination to refrain from smoking may help to quit successfully. So, *after* this session, I advise you to take some time to think of a personal rule that helps you to refrain from smoking. Possible examples include "Not a puff - no matter what,” "Say no to smoking, yes to life" or "Smoking is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
+  </si>
+  <si>
+    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, *after* this session, I advise you to watch the 12-minute video that I will send you as a message in Prolific. The video explains how the body starts repairing itself immediately, as soon as a person stops smoking. What information from the video is most relevant to you? Take a few notes.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for becoming more physically active is to remove possible obstacles. Thus, *after* this session, I advise you to think about things that make it difficult for you to be physically active. For example, this could be that you do NOT have a raincoat to bike to the grocery store when it is raining, that you do NOT want to work out alone, or that you are at work all day and too exhausted by the time that you come home. What are possible solutions to your barriers? For instance, you could buy a raincoat, join a running group, or take a walk during your lunch break at work. Please write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have a strong desire to become more physically active. Therefore, *after* this session, I advise you to identify and write down reasons why you want to become more physically active. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, *after* this session, I advise you to watch the 2-minute video that I will send you as a message in Prolific. The video explains how much and which type of physical activity is recommended. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for this is to have high ambition to become more physically active. Thus, *after* this session, I advise you to think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, *after* this session, I advise you to think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Write down everything that comes to your mind. </t>
+  </si>
+  <si>
+    <t>It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, *after* this session, I advise you to think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Then, look for a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for this is to focus on the goal of becoming more physically active. Thus, *after* this session, I advise you to take some time to visualize becoming more physically active as a battle. For example, you might see yourself and non-active version of yourself as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high motivation to become more physically active. Thus, *after* this session, I advise you to think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Then look for a picture that best captures your desired future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, *after* this session, I advise you to think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, *after* this session, I advise you to watch the 5-minute video that I will send you as a message in Prolific. The video explains the possible positive impact of physical activity on dealing with cravings to smoke. What do you think about the information in the video? Write down your thoughts in a few words.</t>
+  </si>
+  <si>
+    <t>Being more physically active (e.g. exercise, take walks, spend less time sitting) may aid you to stop smoking. One important aspect for this is to have strong resolve to become more physically active. So, *after* this session, I recommend that you take some time to think of a personal rule that helps you to become more physically active. Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may make it easier to successfully quit smoking. One important step for becoming more physically active is to know one's current level. This allows to later set a precise goal and hence to feel more motivated. So, I advise you to record your current behavior with regards to physical activity *after* this session. Try to keep track of how much time you spend 1) sitting, 2) working out and 3) being moderately active (e.g. taking a walk, biking to the grocery store). For this, it might be helpful to keep a piece of paper and pen on your kitchen table, or maybe you have a smart watch that can record these types of behavior for you.</t>
+  </si>
+  <si>
+    <t>Preparing for situations in which you commonly smoke may make it easier to successfully quit smoking. Therefore, I recommend that you record the situations in which you smoke *after* this session. Take note of one or two keywords to describe the situation and the number of cigarettes that you smoked. For example, you might note "Lunch break, 2 cigarettes" or "TV, 5 cigarettes." It might be helpful to take these notes on your phone, or you could carry a small piece of paper and pen in your pocket.</t>
+  </si>
+  <si>
+    <t>Having high aspiration to quit smoking may aid quitting successfully. Thus, before the next session, I advise you to think about the person that you would like to be once you have successfully quit smoking. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Having high aspiration to quit smoking may aid quitting successfully. So, before the next session, I advise you to identify and write down reasons why you want to stop smoking. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Having high motivation to quit smoking may aid quitting successfully. Thus, before the next session, I advise you to think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Write down everything that comes to your mind. </t>
+  </si>
+  <si>
+    <t>Having high motivation to quit smoking may help to quit successfully. So, before the next session, I advise you to think about who you do NOT want to be in the future but might become if you continue to smoke. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her mother did" or a "husband who is frowned upon by his wife" or a "man who is dependent on a substance." Then, look for or take a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Focusing on your goal of successfully quitting smoking may help to quit. Thus, before the next session, I advise you to take some time to visualize smoking as a battle. For example, you might see yourself and a cigarette as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
+  </si>
+  <si>
+    <t>Getting fewer cravings to smoke may make it easier to successfully quit smoking. Therefore, before the next session, I advise you to think about routines in your daily life that often cause you to get cravings to smoke. For example, you might have experienced that if you go to bed very late and thus sleep less, you smoke more the next day. Or maybe you have noticed that if you skip your breakfast, you always smoke on your way to work but NOT otherwise. How could you change these routines to reduce or even avoid those cravings? Please write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Preparing for situations in which avoiding to smoke is difficult may make it easier to successfully quit smoking. Thus, before the next session, I advise you to think about situations in which you might find it difficult to refrain from smoking. For example, this could be during your lunch break at work, when you meet your best friend, or when you watch TV. How could you deal with these situations so that you do NOT smoke? Write down your plans in a few words.</t>
+  </si>
+  <si>
+    <t>Planning how to resist urges to smoke may make it easier to successfully quit smoking. Therefore, before the next session, I advise you to think of activities that you could do to keep yourself busy when you feel the urge to smoke so that you do NOT smoke. These urges typically last a few minutes; think of something that you could do in the meantime until the urge has passed. For example, you could water your plants, eat a carrot, do 10 push-ups, or do something for another person in need. Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Tensing and relaxing areas of the body can reduce cravings and withdrawal symptoms, because it is very difficult to feel tense or uptight in a relaxed body. Thus, before the next session, I advise you to watch the following 15-minute video to learn progressive muscle relaxation (which is a way of relaxing your body): https://www.youtube.com/watch?v=ihO02wUzgkc&amp;ab_channel=MarkConnelly. Even if you have already heard of this technique, it might be a good idea to refresh your memory.</t>
+  </si>
+  <si>
+    <t>Having strong determination to refrain from smoking may help to quit successfully. So, before the next session, I advise you to take some time to think of a personal rule that helps you to refrain from smoking. Possible examples include "Not a puff - no matter what,” "Say no to smoking, yes to life" or "Smoking is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
+  </si>
+  <si>
+    <t>Having a strong desire to refrain from smoking may aid quitting successfully. Thus, before the next session, I advise you to watch the following 12-minute video on how the body starts repairing itself immediately, as soon as a person stops smoking: https://www.youtube.com/watch?v=ZhTOC0T3P3c&amp;ab_channel=RespiratoryTherapyZone. What information from the video is most relevant to you? Take a few notes.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for becoming more physically active is to remove possible obstacles. Thus, before the next session, I advise you to think about things that make it difficult for you to be physically active. For example, this could be that you do NOT have a raincoat to bike to the grocery store when it is raining, that you do NOT want to work out alone, or that you are at work all day and too exhausted by the time that you come home. What are possible solutions to your barriers? For instance, you could buy a raincoat, join a running group, or take a walk during your lunch break at work. Please write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have a strong desire to become more physically active. Therefore, before the next session, I advise you to identify and write down reasons why you want to become more physically active. After writing them down, think about which reasons are most important to you and order them accordingly.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for becoming more physically active is to set a specific goal and thus to feel more aspiration. Therefore, before the next session, I advise you to watch the following 2-minute video on how much and which type of physical activity is recommended: https://www.youtube.com/watch?v=AAPhWbG_zLs&amp;ab_channel=TREKGroup. Then, compare your physical activity behavior to the recommended amounts for the different types of physical activity. Write down which recommended amounts you meet or exceed, and which ones you do NOT meet.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One important step for this is to have high ambition to become more physically active. Thus, before the next session, I advise you to think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, before the next session, I advise you to think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Write down everything that comes to your mind. </t>
+  </si>
+  <si>
+    <t>It may be easier to successfully quit smoking if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high determination to become more physically active. Therefore, before the next session, I advise you to think about who you do NOT want to be in the future but might become if you fail to become more physically active. For example, you might NOT want to be a "mother who dies early of coronary heart disease like her father did" or a "daughter who is frowned upon by her mother" or a "man who is dependent on his wife in his everyday life." Then, look for a picture that best captures your feared future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One important step for this is to focus on the goal of becoming more physically active. Thus, before the next session, I advise you to take some time to visualize becoming more physically active as a battle. For example, you might see yourself and non-active version of yourself as two boxers in a fighting match. Then imagine yourself winning this battle. Visualize clearly how you win and what it feels like to be the winner. Write down a few words about your winning experience.</t>
+  </si>
+  <si>
+    <t>Quitting smoking may be easier if you become more physically active (e.g. exercise, take walks, sit less). One crucial step for this is to have high motivation to become more physically active. Thus, before the next session, I advise you to think about the person that you would like to be once you have become more physically active. For example, you might want to be a "grandfather who can play football with his grandchildren" or a "nurse who can walk up the stairs to the fourth floor without getting out of breath." Then look for a picture that best captures your desired future self. Save or print this picture so that you can see it every day.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may help you to successfully quit smoking. One crucial part for this is to create a plan for becoming more physically active. Therefore, before the next session, I advise you to think about what you could do to become more physically active. For example, you could get up from your desk after every 30 minutes of sitting, bike to the grocery store, do 10 squats every morning, or join a running group. Write down everything that comes to your mind. Which plan do you want to focus on? Highlight this plan.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, spend less time sitting) may help you to successfully quit smoking. One crucial step for this is to have high aspiration to become more physically active. So, before the next session, I advise you to watch the following 5-minute video about the possible positive impact of physical activity on dealing with cravings to smoke: https://www.youtube.com/watch?v=StM10jzbt1k&amp;ab_channel=TreeHouseRecovery. What do you think about the information in the video? Write down your thoughts in a few words.</t>
+  </si>
+  <si>
+    <t>Being more physically active (e.g. exercise, take walks, spend less time sitting) may aid you to stop smoking. One important aspect for this is to have strong resolve to become more physically active. So, before the next session, I advise you to take some time to think of a personal rule that helps you to become more physically active. Possible examples include "10 squats - no matter what," "Say no to sitting, yes to life" or "Driving to the grocery store is NOT an option." Write down your rule on a piece of paper and repeat it to yourself 3 times. Put the piece of paper with your rule somewhere you can see it every day.</t>
+  </si>
+  <si>
+    <t>Preparing for situations in which you commonly smoke may make it easier to successfully quit smoking. Therefore, I recommend that you record the situations in which you smoke before the next session. Take note of one or two keywords to describe the situation and the number of cigarettes that you smoked. For example, you might note "Lunch break, 2 cigarettes" or "TV, 5 cigarettes." It might be helpful to take these notes on your phone, or you could carry a small piece of paper and pen in your pocket.</t>
+  </si>
+  <si>
+    <t>Becoming more physically active (e.g. exercise, take walks, sit less) may make it easier to successfully quit smoking. One important step for becoming more physically active is to know one's current level. This allows to later set a precise goal and hence to feel more motivated. So, I recommend that you record your current behavior with regards to physical activity before the next session. Try to keep track of how much time you spend 1) sitting, 2) working out and 3) being moderately active (e.g. taking a walk, biking to the grocery store). For this, it might be helpful to keep a piece of paper and pen on your kitchen table, or maybe you have a smart watch that can record these types of behavior for you.</t>
   </si>
 </sst>
 </file>
@@ -864,7 +864,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1042,6 +1042,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1205,11 +1211,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1568,7 +1578,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1578,62 +1588,62 @@
     <col min="19" max="19" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1682,13 +1692,13 @@
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>221</v>
+        <v>173</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>27</v>
@@ -1740,10 +1750,10 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>27</v>
@@ -1794,13 +1804,13 @@
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>222</v>
+        <v>174</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>194</v>
+        <v>212</v>
       </c>
       <c r="S4" s="1" t="s">
         <v>27</v>
@@ -1851,13 +1861,13 @@
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>223</v>
+        <v>175</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="S5" s="1" t="s">
         <v>27</v>
@@ -1908,13 +1918,13 @@
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>233</v>
+        <v>185</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="S6" s="1" t="s">
         <v>27</v>
@@ -1968,10 +1978,10 @@
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>191</v>
+        <v>215</v>
       </c>
       <c r="S7" s="1" t="s">
         <v>27</v>
@@ -2025,10 +2035,10 @@
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>190</v>
+        <v>216</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>27</v>
@@ -2080,10 +2090,10 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="S9" s="1" t="s">
         <v>27</v>
@@ -2137,10 +2147,10 @@
         <v>141</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>27</v>
@@ -2194,10 +2204,10 @@
         <v>112</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>187</v>
+        <v>219</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>27</v>
@@ -2248,19 +2258,19 @@
       </c>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>224</v>
+        <v>176</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>186</v>
+        <v>220</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -2306,10 +2316,10 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>185</v>
+        <v>232</v>
       </c>
       <c r="S13" s="1" t="s">
         <v>27</v>
@@ -2359,10 +2369,10 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>184</v>
+        <v>233</v>
       </c>
       <c r="S14" s="1" t="s">
         <v>89</v>
@@ -2412,10 +2422,10 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>183</v>
+        <v>221</v>
       </c>
       <c r="S15" s="1" t="s">
         <v>89</v>
@@ -2467,10 +2477,10 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>182</v>
+        <v>222</v>
       </c>
       <c r="S16" s="1" t="s">
         <v>89</v>
@@ -2521,13 +2531,13 @@
         <v>49</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>225</v>
+        <v>177</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>212</v>
+        <v>199</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>173</v>
+        <v>223</v>
       </c>
       <c r="S17" s="1" t="s">
         <v>89</v>
@@ -2576,13 +2586,13 @@
       </c>
       <c r="O18" s="1"/>
       <c r="P18" s="1" t="s">
-        <v>226</v>
+        <v>178</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>174</v>
+        <v>224</v>
       </c>
       <c r="S18" s="1" t="s">
         <v>89</v>
@@ -2631,13 +2641,13 @@
       </c>
       <c r="O19" s="1"/>
       <c r="P19" s="1" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="S19" s="1" t="s">
         <v>89</v>
@@ -2686,13 +2696,13 @@
       </c>
       <c r="O20" s="1"/>
       <c r="P20" s="1" t="s">
-        <v>228</v>
+        <v>180</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="S20" s="1" t="s">
         <v>89</v>
@@ -2741,13 +2751,13 @@
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="1" t="s">
-        <v>232</v>
+        <v>184</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>177</v>
+        <v>227</v>
       </c>
       <c r="S21" s="1" t="s">
         <v>89</v>
@@ -2796,13 +2806,13 @@
       </c>
       <c r="O22" s="1"/>
       <c r="P22" s="1" t="s">
-        <v>229</v>
+        <v>181</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>217</v>
+        <v>204</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>178</v>
+        <v>228</v>
       </c>
       <c r="S22" s="1" t="s">
         <v>89</v>
@@ -2852,10 +2862,10 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1" t="s">
-        <v>218</v>
+        <v>205</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="S23" s="1" t="s">
         <v>89</v>
@@ -2904,19 +2914,19 @@
       </c>
       <c r="O24" s="1"/>
       <c r="P24" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="R24" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="S24" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2959,13 +2969,13 @@
       </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="R25" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="S25" s="1" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
make clear which activity is about smoking vs PA
</commit_message>
<xml_diff>
--- a/Activities.xlsx
+++ b/Activities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\CAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C6E2BD-EB92-4A54-80D4-81CA03DBE19F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85563382-571E-4CDD-880A-3EAA508E9FEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="273">
   <si>
     <t>Number</t>
   </si>
@@ -73,18 +73,6 @@
     <t>Smoking</t>
   </si>
   <si>
-    <t>thinking about your desired future self</t>
-  </si>
-  <si>
-    <t>Thinking about your desired future self</t>
-  </si>
-  <si>
-    <t>think about your desired future self</t>
-  </si>
-  <si>
-    <t>think about my desired future self</t>
-  </si>
-  <si>
     <t>Thinking about the person you would like to be once you have quit smoking</t>
   </si>
   <si>
@@ -130,18 +118,6 @@
     <t>thinking about who you do NOT want to be but might become if you continue to smoke</t>
   </si>
   <si>
-    <t>thinking about your feared future self</t>
-  </si>
-  <si>
-    <t>Thinking about your feared future self</t>
-  </si>
-  <si>
-    <t>think about your feared future self</t>
-  </si>
-  <si>
-    <t>think about my feared future self</t>
-  </si>
-  <si>
     <t>Thinking about who you do NOT want to be but might become if you continue to smoke</t>
   </si>
   <si>
@@ -259,9 +235,6 @@
     <t>become more physically active</t>
   </si>
   <si>
-    <t>thinking about solutions to possible barriers</t>
-  </si>
-  <si>
     <t>thinking about solutions to barriers</t>
   </si>
   <si>
@@ -271,12 +244,6 @@
     <t>think about solutions to barriers</t>
   </si>
   <si>
-    <t>Thinking about solutions to possible barriers</t>
-  </si>
-  <si>
-    <t>think about solutions to possible barriers</t>
-  </si>
-  <si>
     <t>REMOVE obstacles to becoming more physically active</t>
   </si>
   <si>
@@ -797,6 +764,81 @@
   </si>
   <si>
     <t>Getting fewer cravings to smoke may make it easier to successfully quit smoking. Therefore, before the next session, I advise you to think about routines in your daily life that often cause you to get cravings to smoke. For example, you might have experienced that if you go to bed very late and thus sleep less, you smoke more the next day. Or maybe you have noticed that if you skip your breakfast, you always smoke on your way to work but NOT otherwise. How could you change these routines to reduce or even avoid those cravings? Write down everything that comes to your mind.</t>
+  </si>
+  <si>
+    <t>thinking about who you want to be once you have quit smoking</t>
+  </si>
+  <si>
+    <t>Thinking about who you want to be once you have quit smoking</t>
+  </si>
+  <si>
+    <t>think about who you want to be once you have quit smoking</t>
+  </si>
+  <si>
+    <t>think about who I want to be once I have quit smoking</t>
+  </si>
+  <si>
+    <t>thinking about your feared future self if you continue to smoke</t>
+  </si>
+  <si>
+    <t>Thinking about your feared future self if you continue to smoke</t>
+  </si>
+  <si>
+    <t>think about your feared future self if you continue to smoke</t>
+  </si>
+  <si>
+    <t>think about my feared future self if I continue to smoke</t>
+  </si>
+  <si>
+    <t>creating a personal rule to NOT smoke</t>
+  </si>
+  <si>
+    <t>Creating a personal rule to NOT smoke</t>
+  </si>
+  <si>
+    <t>create a personal rule to NOT smoke</t>
+  </si>
+  <si>
+    <t>thinking about solutions to possible barriers to becoming more physically active</t>
+  </si>
+  <si>
+    <t>Thinking about solutions to possible barriers to becoming more physically active</t>
+  </si>
+  <si>
+    <t>think about solutions to possible barriers to becoming more physically active</t>
+  </si>
+  <si>
+    <t>thinking about who you want to be once you have become more physically active</t>
+  </si>
+  <si>
+    <t>Thinking about who you want to be once you have become more physically active</t>
+  </si>
+  <si>
+    <t>think about who you want to be once you have become more physically active</t>
+  </si>
+  <si>
+    <t>think about who I want to be once I have become more physically active</t>
+  </si>
+  <si>
+    <t>thinking about your feared future self if you do not become more physically active</t>
+  </si>
+  <si>
+    <t>Thinking about your feared future self if you do not become more physically active</t>
+  </si>
+  <si>
+    <t>think about your feared future self if you do not become more physically active</t>
+  </si>
+  <si>
+    <t>think about my feared future self if I do not become more physically active</t>
+  </si>
+  <si>
+    <t>creating a personal rule to become more physically active</t>
+  </si>
+  <si>
+    <t>Creating a personal rule to become more physically active</t>
+  </si>
+  <si>
+    <t>create a personal rule to become more physically active</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1334,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1305,6 +1347,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1664,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P6" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1684,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1726,13 +1771,13 @@
         <v>14</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>15</v>
@@ -1746,56 +1791,56 @@
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
@@ -1806,54 +1851,54 @@
         <v>16</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="187.2" x14ac:dyDescent="0.3">
@@ -1864,56 +1909,56 @@
         <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>36</v>
+        <v>252</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>37</v>
+        <v>253</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>38</v>
+        <v>254</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>39</v>
+        <v>255</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="1" customFormat="1" ht="216" x14ac:dyDescent="0.3">
@@ -1924,56 +1969,56 @@
         <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>36</v>
+        <v>252</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>37</v>
+        <v>253</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>38</v>
+        <v>254</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>39</v>
+        <v>255</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="L5" s="5" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="N5" s="5" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="158.4" x14ac:dyDescent="0.3">
@@ -1984,56 +2029,56 @@
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="1" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
@@ -2044,56 +2089,56 @@
         <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="P7" s="5"/>
       <c r="Q7" s="5" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="187.2" x14ac:dyDescent="0.3">
@@ -2104,56 +2149,56 @@
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="1" customFormat="1" ht="216" x14ac:dyDescent="0.3">
@@ -2164,54 +2209,54 @@
         <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="201.6" x14ac:dyDescent="0.3">
@@ -2222,56 +2267,56 @@
         <v>16</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="1" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
@@ -2282,56 +2327,56 @@
         <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>57</v>
+        <v>256</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>58</v>
+        <v>257</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>59</v>
+        <v>258</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>59</v>
+        <v>258</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="5" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="Q11" s="5" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="S11" s="5" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="T11" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="172.8" x14ac:dyDescent="0.3">
@@ -2342,56 +2387,56 @@
         <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="M12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="1" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
@@ -2402,54 +2447,54 @@
         <v>16</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N13" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>147</v>
       </c>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -2457,55 +2502,55 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:20" s="1" customFormat="1" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -2513,55 +2558,55 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>79</v>
+        <v>259</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>83</v>
+        <v>260</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>84</v>
+        <v>261</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>84</v>
+        <v>261</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="172.8" x14ac:dyDescent="0.3">
@@ -2569,57 +2614,57 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>88</v>
-      </c>
       <c r="G16" s="4" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
@@ -2627,59 +2672,59 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="K17" s="5" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="S17" s="5" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="230.4" x14ac:dyDescent="0.3">
@@ -2687,57 +2732,57 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>18</v>
+        <v>263</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>19</v>
+        <v>264</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>20</v>
+        <v>265</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="1" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
@@ -2745,57 +2790,57 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>36</v>
+        <v>266</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>37</v>
+        <v>267</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>38</v>
+        <v>268</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>39</v>
+        <v>269</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="O19" s="5"/>
       <c r="P19" s="5" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="S19" s="5" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="288" x14ac:dyDescent="0.3">
@@ -2803,57 +2848,57 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>39</v>
+        <v>97</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>269</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="S20" s="4" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:20" s="1" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
@@ -2861,57 +2906,57 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="L21" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L21" s="5" t="s">
-        <v>148</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="O21" s="5"/>
       <c r="P21" s="5" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="S21" s="5" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="T21" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="259.2" x14ac:dyDescent="0.3">
@@ -2919,57 +2964,57 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>17</v>
+        <v>262</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>18</v>
+        <v>263</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>19</v>
+        <v>264</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>20</v>
+        <v>265</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:20" s="1" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
@@ -2977,57 +3022,57 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="K23" s="5" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="P23" s="5"/>
       <c r="Q23" s="5" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="230.4" x14ac:dyDescent="0.3">
@@ -3035,57 +3080,57 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:20" s="1" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
@@ -3093,57 +3138,57 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>57</v>
+        <v>270</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>58</v>
+        <v>271</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>59</v>
+        <v>272</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>59</v>
+        <v>272</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="O25" s="5"/>
       <c r="P25" s="5" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="Q25" s="5" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="S25" s="5" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="T25" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix feared future self formulation
</commit_message>
<xml_diff>
--- a/Activities.xlsx
+++ b/Activities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\CA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85563382-571E-4CDD-880A-3EAA508E9FEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D83ADD-F2E3-4A1F-A075-3DC4C0F6A5ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -778,18 +778,6 @@
     <t>think about who I want to be once I have quit smoking</t>
   </si>
   <si>
-    <t>thinking about your feared future self if you continue to smoke</t>
-  </si>
-  <si>
-    <t>Thinking about your feared future self if you continue to smoke</t>
-  </si>
-  <si>
-    <t>think about your feared future self if you continue to smoke</t>
-  </si>
-  <si>
-    <t>think about my feared future self if I continue to smoke</t>
-  </si>
-  <si>
     <t>creating a personal rule to NOT smoke</t>
   </si>
   <si>
@@ -820,18 +808,6 @@
     <t>think about who I want to be once I have become more physically active</t>
   </si>
   <si>
-    <t>thinking about your feared future self if you do not become more physically active</t>
-  </si>
-  <si>
-    <t>Thinking about your feared future self if you do not become more physically active</t>
-  </si>
-  <si>
-    <t>think about your feared future self if you do not become more physically active</t>
-  </si>
-  <si>
-    <t>think about my feared future self if I do not become more physically active</t>
-  </si>
-  <si>
     <t>creating a personal rule to become more physically active</t>
   </si>
   <si>
@@ -839,6 +815,30 @@
   </si>
   <si>
     <t>create a personal rule to become more physically active</t>
+  </si>
+  <si>
+    <t>thinking about the feared future self you might become if you fail to become more physically active</t>
+  </si>
+  <si>
+    <t>Thinking about the feared future self you might become if you fail to become more physically active</t>
+  </si>
+  <si>
+    <t>think about the feared future self you might become if you fail to become more physically active</t>
+  </si>
+  <si>
+    <t>think about the feared future self I might become if I fail to become more physically active</t>
+  </si>
+  <si>
+    <t>Thinking about the feared future self you might become if you continue to smoke</t>
+  </si>
+  <si>
+    <t>thinking about the feared future self you might become if you continue to smoke</t>
+  </si>
+  <si>
+    <t>think about the feared future self you might become if you continue to smoke</t>
+  </si>
+  <si>
+    <t>think about the feared future self I might become if I continue to smoke</t>
   </si>
 </sst>
 </file>
@@ -1709,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1915,16 +1915,16 @@
         <v>31</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>32</v>
@@ -1975,16 +1975,16 @@
         <v>31</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>32</v>
@@ -2330,7 +2330,7 @@
         <v>125</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>49</v>
@@ -2345,13 +2345,13 @@
         <v>51</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>52</v>
@@ -2564,7 +2564,7 @@
         <v>126</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>71</v>
@@ -2579,13 +2579,13 @@
         <v>73</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>74</v>
@@ -2741,16 +2741,16 @@
         <v>91</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>92</v>
@@ -2799,16 +2799,16 @@
         <v>97</v>
       </c>
       <c r="E19" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="G19" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>269</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>98</v>
@@ -2857,16 +2857,16 @@
         <v>97</v>
       </c>
       <c r="E20" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="F20" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="G20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>269</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>98</v>
@@ -2973,16 +2973,16 @@
         <v>91</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="I22" s="4" t="s">
         <v>92</v>
@@ -3144,7 +3144,7 @@
         <v>126</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>49</v>
@@ -3159,13 +3159,13 @@
         <v>51</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="L25" s="5" t="s">
         <v>117</v>

</xml_diff>

<commit_message>
Make references in activities excel file clearer
</commit_message>
<xml_diff>
--- a/Activities.xlsx
+++ b/Activities.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\CA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nele2\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D83ADD-F2E3-4A1F-A075-3DC4C0F6A5ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41ED645-1E42-4152-A1F1-F7AC2D53212A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>increase your ASPIRATION to move away from smoking</t>
   </si>
   <si>
-    <t>Paper by Eline: "strengthening ideal and future selves among smokers who want to quit"</t>
-  </si>
-  <si>
     <t>may lead to INSUFFICIENT aspiration to move away from smoking</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t>record my current smoking behavior</t>
   </si>
   <si>
-    <t>None, but helps for the activities that ask to come up with routines etc.</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
@@ -839,6 +833,12 @@
   </si>
   <si>
     <t>think about the feared future self I might become if I continue to smoke</t>
+  </si>
+  <si>
+    <t>Paper by Meijer et al.</t>
+  </si>
+  <si>
+    <t>Helps for the activities that ask to come up with routines etc.</t>
   </si>
 </sst>
 </file>
@@ -1709,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1729,7 +1729,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1771,13 +1771,13 @@
         <v>14</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>15</v>
@@ -1791,22 +1791,22 @@
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>249</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>251</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>17</v>
@@ -1821,26 +1821,26 @@
         <v>20</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="O2" s="4"/>
       <c r="P2" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="1" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
@@ -1851,54 +1851,54 @@
         <v>16</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>29</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
       <c r="Q3" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="187.2" x14ac:dyDescent="0.3">
@@ -1909,56 +1909,56 @@
         <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="J4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>144</v>
       </c>
       <c r="O4" s="4"/>
       <c r="P4" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:20" s="1" customFormat="1" ht="216" x14ac:dyDescent="0.3">
@@ -1969,56 +1969,56 @@
         <v>16</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="G5" s="5" t="s">
+      <c r="J5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>144</v>
       </c>
       <c r="O5" s="5"/>
       <c r="P5" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="T5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="158.4" x14ac:dyDescent="0.3">
@@ -2029,56 +2029,56 @@
         <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="G6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" s="4" t="s">
+      <c r="M6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="1" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
@@ -2089,56 +2089,56 @@
         <v>16</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="H7" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="I7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>131</v>
-      </c>
       <c r="O7" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P7" s="5"/>
       <c r="Q7" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="187.2" x14ac:dyDescent="0.3">
@@ -2149,56 +2149,56 @@
         <v>16</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="G8" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>242</v>
-      </c>
       <c r="J8" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="1" customFormat="1" ht="216" x14ac:dyDescent="0.3">
@@ -2209,54 +2209,54 @@
         <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="S9" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="201.6" x14ac:dyDescent="0.3">
@@ -2267,56 +2267,56 @@
         <v>16</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="G10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="L10" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="O10" s="4"/>
       <c r="P10" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:20" s="1" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
@@ -2327,56 +2327,56 @@
         <v>16</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="5" t="s">
+      <c r="K11" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="L11" s="5" t="s">
+      <c r="M11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="O11" s="5"/>
       <c r="P11" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q11" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="S11" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="R11" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>225</v>
-      </c>
       <c r="T11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="172.8" x14ac:dyDescent="0.3">
@@ -2387,56 +2387,56 @@
         <v>16</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="J12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="4" t="s">
+      <c r="M12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="O12" s="4"/>
       <c r="P12" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="1" customFormat="1" ht="201.6" x14ac:dyDescent="0.3">
@@ -2447,54 +2447,54 @@
         <v>16</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="G13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="L13" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>68</v>
+        <v>272</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
       <c r="Q13" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="273.60000000000002" x14ac:dyDescent="0.3">
@@ -2502,55 +2502,55 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="I14" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>148</v>
-      </c>
       <c r="L14" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:20" s="1" customFormat="1" ht="302.39999999999998" x14ac:dyDescent="0.3">
@@ -2558,55 +2558,55 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="F15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="J15" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="5" t="s">
+      <c r="K15" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="L15" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>74</v>
       </c>
       <c r="M15" s="5"/>
       <c r="N15" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="S15" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="T15" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="172.8" x14ac:dyDescent="0.3">
@@ -2614,57 +2614,57 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="H16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="L16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="M16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:20" s="1" customFormat="1" ht="288" x14ac:dyDescent="0.3">
@@ -2672,59 +2672,59 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="G17" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="H17" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="K17" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="J17" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="L17" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="Q17" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="S17" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="T17" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="230.4" x14ac:dyDescent="0.3">
@@ -2732,57 +2732,57 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="I18" s="4" t="s">
+      <c r="K18" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="L18" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="1" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
@@ -2790,57 +2790,57 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="J19" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="I19" s="5" t="s">
+      <c r="K19" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="L19" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>101</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O19" s="5"/>
       <c r="P19" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q19" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="S19" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="T19" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="288" x14ac:dyDescent="0.3">
@@ -2848,57 +2848,57 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J20" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="I20" s="4" t="s">
+      <c r="K20" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q20" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="S20" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="R20" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="S20" s="4" t="s">
-        <v>213</v>
-      </c>
       <c r="T20" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:20" s="1" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
@@ -2906,57 +2906,57 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="H21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J21" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="K21" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>106</v>
-      </c>
       <c r="L21" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M21" s="5"/>
       <c r="N21" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="O21" s="5"/>
       <c r="P21" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q21" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="R21" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="S21" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="T21" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="259.2" x14ac:dyDescent="0.3">
@@ -2964,57 +2964,57 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="I22" s="4" t="s">
+      <c r="K22" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J22" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>94</v>
-      </c>
       <c r="L22" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Q22" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="S22" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="R22" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="S22" s="4" t="s">
-        <v>217</v>
-      </c>
       <c r="T22" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:20" s="1" customFormat="1" ht="230.4" x14ac:dyDescent="0.3">
@@ -3022,57 +3022,57 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="H23" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F23" s="5" t="s">
+      <c r="K23" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="L23" s="5" t="s">
         <v>111</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="L23" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P23" s="5"/>
       <c r="Q23" s="5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="S23" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="T23" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="230.4" x14ac:dyDescent="0.3">
@@ -3080,57 +3080,57 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>141</v>
-      </c>
       <c r="I24" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:20" s="1" customFormat="1" ht="259.2" x14ac:dyDescent="0.3">
@@ -3138,57 +3138,57 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="J25" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="E25" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>264</v>
-      </c>
       <c r="K25" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M25" s="5"/>
       <c r="N25" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="O25" s="5"/>
       <c r="P25" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="Q25" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="R25" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="S25" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="R25" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="S25" s="5" t="s">
-        <v>230</v>
-      </c>
       <c r="T25" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>